<commit_message>
update ons, cbo, uscb
</commit_message>
<xml_diff>
--- a/data-raw/uscb_ae.xlsx
+++ b/data-raw/uscb_ae.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\ADC-IPHS\ISB\CPS\MARCH\2022\P60-276 Income Report\Tables\For PIO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\mar23cps\for_dis\from_inc\Report page- tables &amp; figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{315D217B-773C-4B13-AEED-FAD68F0DDE3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B2B2E9-BE5F-496B-B566-EA2BD1E99C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="tableA5" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">tableA5!$A$1:$O$88</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">tableA5!$A$1:$O$89</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
@@ -48,7 +48,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Selected Measures of Equivalence-Adjusted Income Dispersion: 1967 to 2021</t>
+      <t>Selected Measures of Equivalence-Adjusted Income Dispersion: 1967 to 2022</t>
     </r>
   </si>
   <si>
@@ -81,7 +81,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, Series P60-204. Information on confidentiality protection, sampling error, nonsampling error, and definitions is available at &lt;https://www2.census.gov/programs-surveys/cps/techdocs/cpsmar22.pdf&gt;)</t>
+      <t>, Series P60-204. Information on confidentiality protection, sampling error, nonsampling error, and definitions is available at &lt;https://www2.census.gov/programs-surveys/cps/techdocs/cpsmar23.pdf&gt;)</t>
     </r>
   </si>
   <si>
@@ -731,7 +731,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>3</t>
+      <t>4</t>
     </r>
     <r>
       <rPr>
@@ -741,7 +741,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> The 2014 CPS ASEC included redesigned questions for income and health insurance coverage. All of the approximately 98,000 addresses were eligible to receive the redesigned set of health insurance coverage questions. The redesigned income questions were implemented to a subsample of these 98,000 addresses using a probability split panel design. Approximately 68,000 addresses were eligible to receive a set of income questions similar to those used in the 2013 CPS ASEC and the remaining 30,000 addresses were eligible to receive the redesigned income questions. The source of these 2013 estimates is the portion of the CPS ASEC sample which received the redesigned income questions, approximately 30,000 addresses.</t>
+      <t xml:space="preserve"> The source of these 2013 estimates is the portion of the CPS ASEC sample that received the income questions consistent with the 2013 CPS ASEC, approximately 68,000 addresses.</t>
     </r>
   </si>
   <si>
@@ -755,7 +755,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>4</t>
+      <t>6</t>
     </r>
     <r>
       <rPr>
@@ -765,7 +765,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> The source of these 2013 estimates is the portion of the CPS ASEC sample which received the income questions consistent with the 2013 CPS ASEC, approximately 68,000 addresses.</t>
+      <t xml:space="preserve"> Data have been revised to reflect a correction to the weights in the 2005 CPS ASEC.</t>
     </r>
   </si>
   <si>
@@ -779,7 +779,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>5</t>
+      <t>7</t>
     </r>
     <r>
       <rPr>
@@ -789,7 +789,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Implementation of 2010 Census-based population controls.</t>
+      <t xml:space="preserve"> Implementation of a 28,000-household sample expansion.</t>
     </r>
   </si>
   <si>
@@ -803,7 +803,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>6</t>
+      <t>8</t>
     </r>
     <r>
       <rPr>
@@ -813,7 +813,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Data have been revised to reflect a correction to the weights in the 2005 CPS ASEC.</t>
+      <t xml:space="preserve"> Implementation of 2000 Census-based population controls.</t>
     </r>
   </si>
   <si>
@@ -827,7 +827,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>7</t>
+      <t>9</t>
     </r>
     <r>
       <rPr>
@@ -837,7 +837,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Implementation of a 28,000 household sample expansion.</t>
+      <t xml:space="preserve"> Full implementation of 1990 Census-based sample design and metropolitan definitions, 7,000-household sample reduction, and revised editing of responses on race.</t>
     </r>
   </si>
   <si>
@@ -851,7 +851,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>8</t>
+      <t>10</t>
     </r>
     <r>
       <rPr>
@@ -861,7 +861,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Implementation of 2000 Census-based population controls.</t>
+      <t xml:space="preserve"> Introduction of 1990 Census-based sample design.</t>
     </r>
   </si>
   <si>
@@ -875,7 +875,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>9</t>
+      <t>11</t>
     </r>
     <r>
       <rPr>
@@ -885,7 +885,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Full implementation of 1990 Census-based sample design and metropolitan definitions, 7,000 household sample reduction, and revised editing of responses on race.</t>
+      <t xml:space="preserve"> Data collection method changed from paper and pencil to computer-assisted interviewing. In addition, the 1994 CPS ASEC was revised to allow for the coding of different income amounts on selected questionnaire items. Limits either increased or decreased in the following categories: earnings limits increased to $999,999; Social Security limits increased to $49,999; Supplemental Security Income and public assistance limits increased to $24,999; veterans' benefits limits increased to $99,999; child support and alimony limits decreased to $49,999.</t>
     </r>
   </si>
   <si>
@@ -899,7 +899,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>10</t>
+      <t>12</t>
     </r>
     <r>
       <rPr>
@@ -909,7 +909,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Introduction of 1990 Census sample design.</t>
+      <t xml:space="preserve"> Implementation of 1990 Census-based population controls.</t>
     </r>
   </si>
   <si>
@@ -923,7 +923,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>11</t>
+      <t>13</t>
     </r>
     <r>
       <rPr>
@@ -933,7 +933,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Data collection method changed from paper and pencil to computer-assisted interviewing. In addition, the 1994 CPS ASEC was revised to allow for the coding of different income amounts on selected questionnaire items. Limits either increased or decreased in the following categories: earnings limits increased to $999,999; social security limits increased to $49,999; supplemental security income and public assistance limits increased to $24,999; veterans' benefits limits increased to $99,999; child support and alimony limits decreased to $49,999.</t>
+      <t xml:space="preserve"> Implementation of a new CPS ASEC processing system.</t>
     </r>
   </si>
   <si>
@@ -947,7 +947,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>12</t>
+      <t>14</t>
     </r>
     <r>
       <rPr>
@@ -957,7 +957,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Implementation of 1990 Census population controls.</t>
+      <t xml:space="preserve"> Recording of amounts for earnings from longest job increased to $299,999. Full implementation of 1980 Census-based sample design.</t>
     </r>
   </si>
   <si>
@@ -971,7 +971,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>13</t>
+      <t>15</t>
     </r>
     <r>
       <rPr>
@@ -981,7 +981,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Implementation of a new CPS ASEC processing system.</t>
+      <t xml:space="preserve"> Implementation of Hispanic population weighting controls and introduction of 1980 Census-based sample design.</t>
     </r>
   </si>
   <si>
@@ -995,7 +995,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>14</t>
+      <t>16</t>
     </r>
     <r>
       <rPr>
@@ -1005,7 +1005,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Recording of amounts for earnings from longest job increased to $299,999. Full implementation of 1980 Census-based sample design.</t>
+      <t xml:space="preserve"> Implementation of 1980 Census-based population controls. Questionnaire expanded to show 27 possible values from 51 possible sources of income.</t>
     </r>
   </si>
   <si>
@@ -1019,7 +1019,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>15</t>
+      <t>17</t>
     </r>
     <r>
       <rPr>
@@ -1029,7 +1029,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Implementation of Hispanic population weighting controls and introduction of 1980 Census-based sample design.</t>
+      <t xml:space="preserve"> First year medians were derived using both Pareto and linear interpolation. Before this year, all medians were derived using linear interpolation.</t>
     </r>
   </si>
   <si>
@@ -1043,7 +1043,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>16</t>
+      <t>18</t>
     </r>
     <r>
       <rPr>
@@ -1053,7 +1053,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Implementation of 1980 Census population controls. Questionnaire expanded to allow the recording of up to 27 possible values from a list of 51 possible sources of income.</t>
+      <t xml:space="preserve"> Some of these estimates were derived using Pareto interpolation and may differ from published data, which were derived using linear interpolation.</t>
     </r>
   </si>
   <si>
@@ -1067,7 +1067,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>17</t>
+      <t>19</t>
     </r>
     <r>
       <rPr>
@@ -1077,7 +1077,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> First year medians were derived using both Pareto and linear interpolation. Before this year, all medians were derived using linear interpolation.</t>
+      <t xml:space="preserve"> Implementation of a new CPS ASEC processing system. Questionnaire expanded to ask 11 income questions.</t>
     </r>
   </si>
   <si>
@@ -1091,7 +1091,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>18</t>
+      <t>20</t>
     </r>
     <r>
       <rPr>
@@ -1101,7 +1101,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Some of these estimates were derived using Pareto interpolation and may differ from published data, which were derived using linear interpolation.</t>
+      <t xml:space="preserve"> Full implementation of 1970 Census-based sample design.</t>
     </r>
   </si>
   <si>
@@ -1115,7 +1115,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>19</t>
+      <t>21</t>
     </r>
     <r>
       <rPr>
@@ -1125,8 +1125,14 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Implementation of a new CPS ASEC processing system. Questionnaire expanded to ask 11 income questions.</t>
-    </r>
+      <t xml:space="preserve"> Introduction of 1970 Census-based sample design and population controls.</t>
+    </r>
+  </si>
+  <si>
+    <t>Note: Some estimates have been slightly revised from previous estimates due to an improved table processing system. Margins of error are available via email at sehsd.isb.list@census.gov.</t>
+  </si>
+  <si>
+    <t>Source: U.S. Census Bureau, Current Population Survey, 1968 to 2023 Annual Social and Economic Supplements (CPS ASEC).</t>
   </si>
   <si>
     <r>
@@ -1139,7 +1145,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>20</t>
+      <t>3</t>
     </r>
     <r>
       <rPr>
@@ -1149,7 +1155,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Full implementation of 1970 Census-based sample design.</t>
+      <t xml:space="preserve"> The 2014 CPS ASEC included redesigned questions for income and health insurance coverage. All of the approximately 98,000 addresses were eligible to receive the redesigned set of health insurance coverage questions. The redesigned income questions were implemented to a subsample of these 98,000 addresses using a probability split panel design. Approximately 68,000 addresses were eligible to receive a set of income questions similar to those used in the 2013 CPS ASEC, and the remaining 30,000 addresses were eligible to receive the redesigned income questions. The source of these 2013 estimates is the portion of the CPS ASEC sample that received the redesigned income questions, approximately 30,000 addresses.</t>
     </r>
   </si>
   <si>
@@ -1163,7 +1169,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>21</t>
+      <t>22</t>
     </r>
     <r>
       <rPr>
@@ -1173,11 +1179,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Introduction of 1970 Census sample design and population controls.</t>
-    </r>
-  </si>
-  <si>
-    <t>Source: U.S. Census Bureau, Current Population Survey, 1968 to 2022 Annual Social and Economic Supplements (CPS ASEC).</t>
+      <t xml:space="preserve"> Implementation of a new CPS ASEC processing system.</t>
+    </r>
   </si>
   <si>
     <r>
@@ -1190,7 +1193,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>22</t>
+      <t>5</t>
     </r>
     <r>
       <rPr>
@@ -1200,11 +1203,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Implementation of a new CPS ASEC processing system.</t>
-    </r>
-  </si>
-  <si>
-    <t>Note: Some estimates have been slightly revised from previous estimates due to an improved table processing system. Margins of error are available via email at &lt;sehsd.isb.list@census.gov&gt;.</t>
+      <t xml:space="preserve"> Implementation of 2010 Census-based population controls.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1729,7 +1729,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O88"/>
+  <dimension ref="A1:O89"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
@@ -1741,7 +1741,7 @@
     <col min="1" max="1" width="9.85546875" customWidth="1"/>
     <col min="2" max="10" width="10.140625" customWidth="1"/>
     <col min="11" max="11" width="11.28515625" customWidth="1"/>
-    <col min="12" max="16" width="10.140625" customWidth="1"/>
+    <col min="12" max="15" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="3" customHeight="1" x14ac:dyDescent="0.25">
@@ -1911,386 +1911,386 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B8" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="C8" s="3">
+        <v>9.1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>14.6</v>
+      </c>
+      <c r="E8" s="3">
+        <v>22.1</v>
+      </c>
+      <c r="F8" s="3">
+        <v>50.7</v>
+      </c>
+      <c r="G8" s="4">
+        <v>10.37</v>
+      </c>
+      <c r="H8" s="4">
+        <v>2.71</v>
+      </c>
+      <c r="I8" s="4">
+        <v>3.82</v>
+      </c>
+      <c r="J8" s="5">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="K8" s="5">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="L8" s="5">
+        <v>0.40799999999999997</v>
+      </c>
+      <c r="M8" s="5">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="N8" s="5">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="O8" s="5">
+        <v>0.30299999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>2021</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B9" s="3">
         <v>3.3</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C9" s="3">
         <v>8.8000000000000007</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D9" s="3">
         <v>14.4</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E9" s="3">
         <v>22.3</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F9" s="3">
         <v>51.2</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G9" s="4">
         <v>10.89</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H9" s="4">
         <v>2.81</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I9" s="4">
         <v>3.88</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J9" s="5">
         <v>0.47399999999999998</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K9" s="5">
         <v>0.66200000000000003</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L9" s="5">
         <v>0.41899999999999998</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M9" s="5">
         <v>0.10100000000000001</v>
       </c>
-      <c r="N8" s="5">
+      <c r="N9" s="5">
         <v>0.19900000000000001</v>
       </c>
-      <c r="O8" s="5">
+      <c r="O9" s="5">
         <v>0.308</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+    <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B10" s="3">
         <v>3.4</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C10" s="3">
         <v>8.9</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D10" s="3">
         <v>14.5</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E10" s="3">
         <v>22.4</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F10" s="3">
         <v>50.8</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G10" s="4">
         <v>10.73</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H10" s="4">
         <v>2.8</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I10" s="4">
         <v>3.83</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J10" s="5">
         <v>0.46899999999999997</v>
       </c>
-      <c r="K9" s="5">
+      <c r="K10" s="5">
         <v>0.64300000000000002</v>
       </c>
-      <c r="L9" s="5">
+      <c r="L10" s="5">
         <v>0.41</v>
       </c>
-      <c r="M9" s="5">
+      <c r="M10" s="5">
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="N9" s="5">
+      <c r="N10" s="5">
         <v>0.19500000000000001</v>
       </c>
-      <c r="O9" s="5">
+      <c r="O10" s="5">
         <v>0.30199999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>2019</v>
-      </c>
-      <c r="B10" s="3">
-        <v>3.6</v>
-      </c>
-      <c r="C10" s="3">
-        <v>9</v>
-      </c>
-      <c r="D10" s="3">
-        <v>14.6</v>
-      </c>
-      <c r="E10" s="3">
-        <v>22.3</v>
-      </c>
-      <c r="F10" s="3">
-        <v>50.5</v>
-      </c>
-      <c r="G10" s="4">
-        <v>9.7799999999999994</v>
-      </c>
-      <c r="H10" s="4">
-        <v>2.71</v>
-      </c>
-      <c r="I10" s="4">
-        <v>3.61</v>
-      </c>
-      <c r="J10" s="5">
-        <v>0.46500000000000002</v>
-      </c>
-      <c r="K10" s="5">
-        <v>0.59699999999999998</v>
-      </c>
-      <c r="L10" s="5">
-        <v>0.40400000000000003</v>
-      </c>
-      <c r="M10" s="5">
-        <v>9.7000000000000003E-2</v>
-      </c>
-      <c r="N10" s="5">
-        <v>0.19</v>
-      </c>
-      <c r="O10" s="5">
-        <v>0.29099999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="B11" s="3">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="C11" s="3">
-        <v>9.1</v>
+        <v>9</v>
       </c>
       <c r="D11" s="3">
-        <v>14.7</v>
+        <v>14.6</v>
       </c>
       <c r="E11" s="3">
-        <v>22.4</v>
+        <v>22.3</v>
       </c>
       <c r="F11" s="3">
-        <v>50.3</v>
+        <v>50.5</v>
       </c>
       <c r="G11" s="4">
-        <v>10.09</v>
+        <v>9.7799999999999994</v>
       </c>
       <c r="H11" s="4">
-        <v>2.7</v>
+        <v>2.71</v>
       </c>
       <c r="I11" s="4">
-        <v>3.74</v>
+        <v>3.61</v>
       </c>
       <c r="J11" s="5">
-        <v>0.46400000000000002</v>
+        <v>0.46500000000000002</v>
       </c>
       <c r="K11" s="5">
-        <v>0.628</v>
+        <v>0.59699999999999998</v>
       </c>
       <c r="L11" s="5">
-        <v>0.40500000000000003</v>
+        <v>0.40400000000000003</v>
       </c>
       <c r="M11" s="5">
         <v>9.7000000000000003E-2</v>
       </c>
       <c r="N11" s="5">
-        <v>0.191</v>
+        <v>0.19</v>
       </c>
       <c r="O11" s="5">
-        <v>0.29599999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>24</v>
+        <v>0.29099999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>2018</v>
       </c>
       <c r="B12" s="3">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="C12" s="3">
-        <v>8.9</v>
+        <v>9.1</v>
       </c>
       <c r="D12" s="3">
-        <v>14.4</v>
+        <v>14.7</v>
       </c>
       <c r="E12" s="3">
         <v>22.4</v>
       </c>
       <c r="F12" s="3">
+        <v>50.3</v>
+      </c>
+      <c r="G12" s="4">
+        <v>10.09</v>
+      </c>
+      <c r="H12" s="4">
+        <v>2.7</v>
+      </c>
+      <c r="I12" s="4">
+        <v>3.74</v>
+      </c>
+      <c r="J12" s="5">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="K12" s="5">
+        <v>0.628</v>
+      </c>
+      <c r="L12" s="5">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="M12" s="5">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="N12" s="5">
+        <v>0.191</v>
+      </c>
+      <c r="O12" s="5">
+        <v>0.29599999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="3">
+        <v>3.4</v>
+      </c>
+      <c r="C13" s="3">
+        <v>8.9</v>
+      </c>
+      <c r="D13" s="3">
+        <v>14.4</v>
+      </c>
+      <c r="E13" s="3">
+        <v>22.4</v>
+      </c>
+      <c r="F13" s="3">
         <v>50.9</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G13" s="4">
         <v>10.59</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H13" s="4">
         <v>2.78</v>
-      </c>
-      <c r="I12" s="4">
-        <v>3.8</v>
-      </c>
-      <c r="J12" s="5">
-        <v>0.47099999999999997</v>
-      </c>
-      <c r="K12" s="5">
-        <v>0.64300000000000002</v>
-      </c>
-      <c r="L12" s="5">
-        <v>0.41599999999999998</v>
-      </c>
-      <c r="M12" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="N12" s="5">
-        <v>0.19600000000000001</v>
-      </c>
-      <c r="O12" s="5">
-        <v>0.30399999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>2017</v>
-      </c>
-      <c r="B13" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="C13" s="3">
-        <v>9</v>
-      </c>
-      <c r="D13" s="3">
-        <v>14.7</v>
-      </c>
-      <c r="E13" s="3">
-        <v>22.7</v>
-      </c>
-      <c r="F13" s="3">
-        <v>50.1</v>
-      </c>
-      <c r="G13" s="4">
-        <v>10.45</v>
-      </c>
-      <c r="H13" s="4">
-        <v>2.75</v>
       </c>
       <c r="I13" s="4">
         <v>3.8</v>
       </c>
       <c r="J13" s="5">
-        <v>0.46300000000000002</v>
+        <v>0.47099999999999997</v>
       </c>
       <c r="K13" s="5">
-        <v>0.63900000000000001</v>
+        <v>0.64300000000000002</v>
       </c>
       <c r="L13" s="5">
-        <v>0.39700000000000002</v>
+        <v>0.41599999999999998</v>
       </c>
       <c r="M13" s="5">
-        <v>9.6000000000000002E-2</v>
+        <v>0.1</v>
       </c>
       <c r="N13" s="5">
-        <v>0.191</v>
+        <v>0.19600000000000001</v>
       </c>
       <c r="O13" s="5">
-        <v>0.29799999999999999</v>
+        <v>0.30399999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="B14" s="3">
         <v>3.5</v>
       </c>
       <c r="C14" s="3">
-        <v>9.1</v>
+        <v>9</v>
       </c>
       <c r="D14" s="3">
         <v>14.7</v>
       </c>
       <c r="E14" s="3">
-        <v>22.5</v>
+        <v>22.7</v>
       </c>
       <c r="F14" s="3">
-        <v>50.2</v>
+        <v>50.1</v>
       </c>
       <c r="G14" s="4">
-        <v>10.38</v>
+        <v>10.45</v>
       </c>
       <c r="H14" s="4">
-        <v>2.7</v>
+        <v>2.75</v>
       </c>
       <c r="I14" s="4">
-        <v>3.84</v>
+        <v>3.8</v>
       </c>
       <c r="J14" s="5">
-        <v>0.46400000000000002</v>
+        <v>0.46300000000000002</v>
       </c>
       <c r="K14" s="5">
-        <v>0.629</v>
+        <v>0.63900000000000001</v>
       </c>
       <c r="L14" s="5">
-        <v>0.40300000000000002</v>
+        <v>0.39700000000000002</v>
       </c>
       <c r="M14" s="5">
-        <v>9.7000000000000003E-2</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="N14" s="5">
-        <v>0.192</v>
+        <v>0.191</v>
       </c>
       <c r="O14" s="5">
-        <v>0.29699999999999999</v>
+        <v>0.29799999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="B15" s="3">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="C15" s="3">
-        <v>9</v>
+        <v>9.1</v>
       </c>
       <c r="D15" s="3">
-        <v>14.8</v>
+        <v>14.7</v>
       </c>
       <c r="E15" s="3">
-        <v>22.9</v>
+        <v>22.5</v>
       </c>
       <c r="F15" s="3">
-        <v>49.8</v>
+        <v>50.2</v>
       </c>
       <c r="G15" s="4">
-        <v>10.48</v>
+        <v>10.38</v>
       </c>
       <c r="H15" s="4">
-        <v>2.68</v>
+        <v>2.7</v>
       </c>
       <c r="I15" s="4">
-        <v>3.92</v>
+        <v>3.84</v>
       </c>
       <c r="J15" s="5">
-        <v>0.46200000000000002</v>
+        <v>0.46400000000000002</v>
       </c>
       <c r="K15" s="5">
-        <v>0.623</v>
+        <v>0.629</v>
       </c>
       <c r="L15" s="5">
-        <v>0.39600000000000002</v>
+        <v>0.40300000000000002</v>
       </c>
       <c r="M15" s="5">
-        <v>9.6000000000000002E-2</v>
+        <v>9.7000000000000003E-2</v>
       </c>
       <c r="N15" s="5">
-        <v>0.19</v>
+        <v>0.192</v>
       </c>
       <c r="O15" s="5">
-        <v>0.29499999999999998</v>
+        <v>0.29699999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="B16" s="3">
-        <v>3.3</v>
+        <v>3.4</v>
       </c>
       <c r="C16" s="3">
         <v>9</v>
@@ -2302,78 +2302,78 @@
         <v>22.9</v>
       </c>
       <c r="F16" s="3">
-        <v>50</v>
+        <v>49.8</v>
       </c>
       <c r="G16" s="4">
-        <v>10.71</v>
+        <v>10.48</v>
       </c>
       <c r="H16" s="4">
-        <v>2.72</v>
+        <v>2.68</v>
       </c>
       <c r="I16" s="4">
-        <v>3.93</v>
+        <v>3.92</v>
       </c>
       <c r="J16" s="5">
-        <v>0.46400000000000002</v>
+        <v>0.46200000000000002</v>
       </c>
       <c r="K16" s="5">
-        <v>0.64800000000000002</v>
+        <v>0.623</v>
       </c>
       <c r="L16" s="5">
-        <v>0.39700000000000002</v>
+        <v>0.39600000000000002</v>
       </c>
       <c r="M16" s="5">
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="N16" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="O16" s="5">
+        <v>0.29499999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>2014</v>
+      </c>
+      <c r="B17" s="3">
+        <v>3.3</v>
+      </c>
+      <c r="C17" s="3">
+        <v>9</v>
+      </c>
+      <c r="D17" s="3">
+        <v>14.8</v>
+      </c>
+      <c r="E17" s="3">
+        <v>22.9</v>
+      </c>
+      <c r="F17" s="3">
+        <v>50</v>
+      </c>
+      <c r="G17" s="4">
+        <v>10.71</v>
+      </c>
+      <c r="H17" s="4">
+        <v>2.72</v>
+      </c>
+      <c r="I17" s="4">
+        <v>3.93</v>
+      </c>
+      <c r="J17" s="5">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="K17" s="5">
+        <v>0.64800000000000002</v>
+      </c>
+      <c r="L17" s="5">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="M17" s="5">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="N17" s="5">
         <v>0.192</v>
-      </c>
-      <c r="O16" s="5">
-        <v>0.30099999999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="3">
-        <v>3.4</v>
-      </c>
-      <c r="C17" s="3">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="D17" s="3">
-        <v>14.7</v>
-      </c>
-      <c r="E17" s="3">
-        <v>22.8</v>
-      </c>
-      <c r="F17" s="3">
-        <v>50.3</v>
-      </c>
-      <c r="G17" s="4">
-        <v>10.65</v>
-      </c>
-      <c r="H17" s="4">
-        <v>2.73</v>
-      </c>
-      <c r="I17" s="4">
-        <v>3.91</v>
-      </c>
-      <c r="J17" s="5">
-        <v>0.46700000000000003</v>
-      </c>
-      <c r="K17" s="5">
-        <v>0.63500000000000001</v>
-      </c>
-      <c r="L17" s="5">
-        <v>0.40899999999999997</v>
-      </c>
-      <c r="M17" s="5">
-        <v>9.8000000000000004E-2</v>
-      </c>
-      <c r="N17" s="5">
-        <v>0.19400000000000001</v>
       </c>
       <c r="O17" s="5">
         <v>0.30099999999999999</v>
@@ -2381,101 +2381,101 @@
     </row>
     <row r="18" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="3">
+        <v>3.4</v>
+      </c>
+      <c r="C18" s="3">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="D18" s="3">
+        <v>14.7</v>
+      </c>
+      <c r="E18" s="3">
+        <v>22.8</v>
+      </c>
+      <c r="F18" s="3">
+        <v>50.3</v>
+      </c>
+      <c r="G18" s="4">
+        <v>10.65</v>
+      </c>
+      <c r="H18" s="4">
+        <v>2.73</v>
+      </c>
+      <c r="I18" s="4">
+        <v>3.91</v>
+      </c>
+      <c r="J18" s="5">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="K18" s="5">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="L18" s="5">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="M18" s="5">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="N18" s="5">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="O18" s="5">
+        <v>0.30099999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B19" s="3">
         <v>3.5</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C19" s="3">
         <v>9.1</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D19" s="3">
         <v>14.9</v>
-      </c>
-      <c r="E18" s="3">
-        <v>22.9</v>
-      </c>
-      <c r="F18" s="3">
-        <v>49.6</v>
-      </c>
-      <c r="G18" s="4">
-        <v>10.09</v>
-      </c>
-      <c r="H18" s="4">
-        <v>2.66</v>
-      </c>
-      <c r="I18" s="4">
-        <v>3.79</v>
-      </c>
-      <c r="J18" s="5">
-        <v>0.45900000000000002</v>
-      </c>
-      <c r="K18" s="5">
-        <v>0.62</v>
-      </c>
-      <c r="L18" s="5">
-        <v>0.39200000000000002</v>
-      </c>
-      <c r="M18" s="5">
-        <v>9.5000000000000001E-2</v>
-      </c>
-      <c r="N18" s="5">
-        <v>0.188</v>
-      </c>
-      <c r="O18" s="5">
-        <v>0.29299999999999998</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>2012</v>
-      </c>
-      <c r="B19" s="3">
-        <v>3.4</v>
-      </c>
-      <c r="C19" s="3">
-        <v>9</v>
-      </c>
-      <c r="D19" s="3">
-        <v>14.8</v>
       </c>
       <c r="E19" s="3">
         <v>22.9</v>
       </c>
       <c r="F19" s="3">
-        <v>49.9</v>
+        <v>49.6</v>
       </c>
       <c r="G19" s="4">
-        <v>10.38</v>
+        <v>10.09</v>
       </c>
       <c r="H19" s="4">
         <v>2.66</v>
       </c>
       <c r="I19" s="4">
-        <v>3.91</v>
+        <v>3.79</v>
       </c>
       <c r="J19" s="5">
-        <v>0.46300000000000002</v>
+        <v>0.45900000000000002</v>
       </c>
       <c r="K19" s="5">
-        <v>0.629</v>
+        <v>0.62</v>
       </c>
       <c r="L19" s="5">
-        <v>0.40500000000000003</v>
+        <v>0.39200000000000002</v>
       </c>
       <c r="M19" s="5">
-        <v>9.7000000000000003E-2</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="N19" s="5">
-        <v>0.192</v>
+        <v>0.188</v>
       </c>
       <c r="O19" s="5">
-        <v>0.29799999999999999</v>
+        <v>0.29299999999999998</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="B20" s="3">
         <v>3.4</v>
@@ -2487,465 +2487,465 @@
         <v>14.8</v>
       </c>
       <c r="E20" s="3">
-        <v>22.8</v>
+        <v>22.9</v>
       </c>
       <c r="F20" s="3">
-        <v>50</v>
+        <v>49.9</v>
       </c>
       <c r="G20" s="4">
-        <v>10.19</v>
+        <v>10.38</v>
       </c>
       <c r="H20" s="4">
-        <v>2.69</v>
+        <v>2.66</v>
       </c>
       <c r="I20" s="4">
-        <v>3.79</v>
+        <v>3.91</v>
       </c>
       <c r="J20" s="5">
         <v>0.46300000000000002</v>
       </c>
       <c r="K20" s="5">
-        <v>0.626</v>
+        <v>0.629</v>
       </c>
       <c r="L20" s="5">
-        <v>0.40400000000000003</v>
+        <v>0.40500000000000003</v>
       </c>
       <c r="M20" s="5">
         <v>9.7000000000000003E-2</v>
       </c>
       <c r="N20" s="5">
-        <v>0.191</v>
+        <v>0.192</v>
       </c>
       <c r="O20" s="5">
-        <v>0.29699999999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>27</v>
+        <v>0.29799999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>2011</v>
       </c>
       <c r="B21" s="3">
         <v>3.4</v>
       </c>
       <c r="C21" s="3">
+        <v>9</v>
+      </c>
+      <c r="D21" s="3">
+        <v>14.8</v>
+      </c>
+      <c r="E21" s="3">
+        <v>22.8</v>
+      </c>
+      <c r="F21" s="3">
+        <v>50</v>
+      </c>
+      <c r="G21" s="4">
+        <v>10.19</v>
+      </c>
+      <c r="H21" s="4">
+        <v>2.69</v>
+      </c>
+      <c r="I21" s="4">
+        <v>3.79</v>
+      </c>
+      <c r="J21" s="5">
+        <v>0.46300000000000002</v>
+      </c>
+      <c r="K21" s="5">
+        <v>0.626</v>
+      </c>
+      <c r="L21" s="5">
+        <v>0.40400000000000003</v>
+      </c>
+      <c r="M21" s="5">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="N21" s="5">
+        <v>0.191</v>
+      </c>
+      <c r="O21" s="5">
+        <v>0.29699999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="3">
+        <v>3.4</v>
+      </c>
+      <c r="C22" s="3">
         <v>9.1999999999999993</v>
-      </c>
-      <c r="D21" s="3">
-        <v>15</v>
-      </c>
-      <c r="E21" s="3">
-        <v>23.1</v>
-      </c>
-      <c r="F21" s="3">
-        <v>49.2</v>
-      </c>
-      <c r="G21" s="4">
-        <v>10.44</v>
-      </c>
-      <c r="H21" s="4">
-        <v>2.67</v>
-      </c>
-      <c r="I21" s="4">
-        <v>3.91</v>
-      </c>
-      <c r="J21" s="5">
-        <v>0.45600000000000002</v>
-      </c>
-      <c r="K21" s="5">
-        <v>0.61699999999999999</v>
-      </c>
-      <c r="L21" s="5">
-        <v>0.38200000000000001</v>
-      </c>
-      <c r="M21" s="5">
-        <v>9.2999999999999999E-2</v>
-      </c>
-      <c r="N21" s="5">
-        <v>0.185</v>
-      </c>
-      <c r="O21" s="5">
-        <v>0.28999999999999998</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>2009</v>
-      </c>
-      <c r="B22" s="3">
-        <v>3.6</v>
-      </c>
-      <c r="C22" s="3">
-        <v>9.3000000000000007</v>
       </c>
       <c r="D22" s="3">
         <v>15</v>
       </c>
       <c r="E22" s="3">
-        <v>22.9</v>
+        <v>23.1</v>
       </c>
       <c r="F22" s="3">
-        <v>49.4</v>
+        <v>49.2</v>
       </c>
       <c r="G22" s="4">
-        <v>10.07</v>
+        <v>10.44</v>
       </c>
       <c r="H22" s="4">
-        <v>2.63</v>
+        <v>2.67</v>
       </c>
       <c r="I22" s="4">
-        <v>3.82</v>
+        <v>3.91</v>
       </c>
       <c r="J22" s="5">
         <v>0.45600000000000002</v>
       </c>
       <c r="K22" s="5">
-        <v>0.60499999999999998</v>
+        <v>0.61699999999999999</v>
       </c>
       <c r="L22" s="5">
-        <v>0.39</v>
+        <v>0.38200000000000001</v>
       </c>
       <c r="M22" s="5">
-        <v>9.4E-2</v>
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="N22" s="5">
-        <v>0.186</v>
+        <v>0.185</v>
       </c>
       <c r="O22" s="5">
-        <v>0.28899999999999998</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="B23" s="3">
-        <v>3.7</v>
+        <v>3.6</v>
       </c>
       <c r="C23" s="3">
-        <v>9.4</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="D23" s="3">
-        <v>15.1</v>
+        <v>15</v>
       </c>
       <c r="E23" s="3">
-        <v>22.8</v>
+        <v>22.9</v>
       </c>
       <c r="F23" s="3">
-        <v>48.9</v>
+        <v>49.4</v>
       </c>
       <c r="G23" s="4">
-        <v>9.5</v>
+        <v>10.07</v>
       </c>
       <c r="H23" s="4">
-        <v>2.58</v>
+        <v>2.63</v>
       </c>
       <c r="I23" s="4">
-        <v>3.68</v>
+        <v>3.82</v>
       </c>
       <c r="J23" s="5">
-        <v>0.45</v>
+        <v>0.45600000000000002</v>
       </c>
       <c r="K23" s="5">
-        <v>0.56799999999999995</v>
+        <v>0.60499999999999998</v>
       </c>
       <c r="L23" s="5">
-        <v>0.377</v>
+        <v>0.39</v>
       </c>
       <c r="M23" s="5">
-        <v>9.0999999999999998E-2</v>
+        <v>9.4E-2</v>
       </c>
       <c r="N23" s="5">
-        <v>0.18</v>
+        <v>0.186</v>
       </c>
       <c r="O23" s="5">
-        <v>0.27800000000000002</v>
+        <v>0.28899999999999998</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="B24" s="3">
-        <v>3.8</v>
+        <v>3.7</v>
       </c>
       <c r="C24" s="3">
+        <v>9.4</v>
+      </c>
+      <c r="D24" s="3">
+        <v>15.1</v>
+      </c>
+      <c r="E24" s="3">
+        <v>22.8</v>
+      </c>
+      <c r="F24" s="3">
+        <v>48.9</v>
+      </c>
+      <c r="G24" s="4">
         <v>9.5</v>
       </c>
-      <c r="D24" s="3">
-        <v>15.3</v>
-      </c>
-      <c r="E24" s="3">
-        <v>22.9</v>
-      </c>
-      <c r="F24" s="3">
-        <v>48.5</v>
-      </c>
-      <c r="G24" s="4">
-        <v>9.19</v>
-      </c>
       <c r="H24" s="4">
-        <v>2.5499999999999998</v>
+        <v>2.58</v>
       </c>
       <c r="I24" s="4">
-        <v>3.6</v>
+        <v>3.68</v>
       </c>
       <c r="J24" s="5">
-        <v>0.44400000000000001</v>
+        <v>0.45</v>
       </c>
       <c r="K24" s="5">
-        <v>0.54800000000000004</v>
+        <v>0.56799999999999995</v>
       </c>
       <c r="L24" s="5">
-        <v>0.36799999999999999</v>
+        <v>0.377</v>
       </c>
       <c r="M24" s="5">
-        <v>8.8999999999999996E-2</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="N24" s="5">
-        <v>0.17499999999999999</v>
+        <v>0.18</v>
       </c>
       <c r="O24" s="5">
-        <v>0.27100000000000002</v>
+        <v>0.27800000000000002</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="B25" s="3">
         <v>3.8</v>
       </c>
       <c r="C25" s="3">
-        <v>9.4</v>
+        <v>9.5</v>
       </c>
       <c r="D25" s="3">
-        <v>14.9</v>
+        <v>15.3</v>
       </c>
       <c r="E25" s="3">
-        <v>22.5</v>
+        <v>22.9</v>
       </c>
       <c r="F25" s="3">
-        <v>49.3</v>
+        <v>48.5</v>
       </c>
       <c r="G25" s="4">
-        <v>9.1199999999999992</v>
+        <v>9.19</v>
       </c>
       <c r="H25" s="4">
-        <v>2.57</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="I25" s="4">
-        <v>3.55</v>
+        <v>3.6</v>
       </c>
       <c r="J25" s="5">
-        <v>0.45200000000000001</v>
+        <v>0.44400000000000001</v>
       </c>
       <c r="K25" s="5">
-        <v>0.55700000000000005</v>
+        <v>0.54800000000000004</v>
       </c>
       <c r="L25" s="5">
-        <v>0.39300000000000002</v>
+        <v>0.36799999999999999</v>
       </c>
       <c r="M25" s="5">
-        <v>9.2999999999999999E-2</v>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="N25" s="5">
-        <v>0.182</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="O25" s="5">
-        <v>0.27800000000000002</v>
+        <v>0.27100000000000002</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>2005</v>
+        <v>2006</v>
       </c>
       <c r="B26" s="3">
         <v>3.8</v>
       </c>
       <c r="C26" s="3">
-        <v>9.5</v>
+        <v>9.4</v>
       </c>
       <c r="D26" s="3">
-        <v>15.1</v>
+        <v>14.9</v>
       </c>
       <c r="E26" s="3">
-        <v>22.6</v>
+        <v>22.5</v>
       </c>
       <c r="F26" s="3">
-        <v>49.1</v>
+        <v>49.3</v>
       </c>
       <c r="G26" s="4">
-        <v>9.27</v>
+        <v>9.1199999999999992</v>
       </c>
       <c r="H26" s="4">
-        <v>2.5499999999999998</v>
+        <v>2.57</v>
       </c>
       <c r="I26" s="4">
-        <v>3.64</v>
+        <v>3.55</v>
       </c>
       <c r="J26" s="5">
-        <v>0.45</v>
+        <v>0.45200000000000001</v>
       </c>
       <c r="K26" s="5">
-        <v>0.57099999999999995</v>
+        <v>0.55700000000000005</v>
       </c>
       <c r="L26" s="5">
-        <v>0.38600000000000001</v>
+        <v>0.39300000000000002</v>
       </c>
       <c r="M26" s="5">
-        <v>9.1999999999999998E-2</v>
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="N26" s="5">
-        <v>0.18099999999999999</v>
+        <v>0.182</v>
       </c>
       <c r="O26" s="5">
-        <v>0.28000000000000003</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
-        <v>28</v>
+        <v>0.27800000000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>2005</v>
       </c>
       <c r="B27" s="3">
         <v>3.8</v>
       </c>
       <c r="C27" s="3">
-        <v>9.6</v>
+        <v>9.5</v>
       </c>
       <c r="D27" s="3">
-        <v>15.2</v>
+        <v>15.1</v>
       </c>
       <c r="E27" s="3">
-        <v>22.7</v>
+        <v>22.6</v>
       </c>
       <c r="F27" s="3">
-        <v>48.7</v>
+        <v>49.1</v>
       </c>
       <c r="G27" s="4">
-        <v>9.2200000000000006</v>
+        <v>9.27</v>
       </c>
       <c r="H27" s="4">
         <v>2.5499999999999998</v>
       </c>
       <c r="I27" s="4">
-        <v>3.62</v>
+        <v>3.64</v>
       </c>
       <c r="J27" s="5">
-        <v>0.44700000000000001</v>
+        <v>0.45</v>
       </c>
       <c r="K27" s="5">
-        <v>0.55900000000000005</v>
+        <v>0.57099999999999995</v>
       </c>
       <c r="L27" s="5">
-        <v>0.38</v>
+        <v>0.38600000000000001</v>
       </c>
       <c r="M27" s="5">
-        <v>9.0999999999999998E-2</v>
+        <v>9.1999999999999998E-2</v>
       </c>
       <c r="N27" s="5">
-        <v>0.17899999999999999</v>
+        <v>0.18099999999999999</v>
       </c>
       <c r="O27" s="5">
-        <v>0.27600000000000002</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <v>2003</v>
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="B28" s="3">
-        <v>3.9</v>
+        <v>3.8</v>
       </c>
       <c r="C28" s="3">
-        <v>9.5</v>
+        <v>9.6</v>
       </c>
       <c r="D28" s="3">
         <v>15.2</v>
       </c>
       <c r="E28" s="3">
-        <v>22.8</v>
+        <v>22.7</v>
       </c>
       <c r="F28" s="3">
-        <v>48.6</v>
+        <v>48.7</v>
       </c>
       <c r="G28" s="4">
-        <v>9.15</v>
+        <v>9.2200000000000006</v>
       </c>
       <c r="H28" s="4">
-        <v>2.56</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="I28" s="4">
-        <v>3.58</v>
+        <v>3.62</v>
       </c>
       <c r="J28" s="5">
-        <v>0.44500000000000001</v>
+        <v>0.44700000000000001</v>
       </c>
       <c r="K28" s="5">
-        <v>0.54800000000000004</v>
+        <v>0.55900000000000005</v>
       </c>
       <c r="L28" s="5">
-        <v>0.373</v>
+        <v>0.38</v>
       </c>
       <c r="M28" s="5">
-        <v>0.09</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="N28" s="5">
-        <v>0.17599999999999999</v>
+        <v>0.17899999999999999</v>
       </c>
       <c r="O28" s="5">
-        <v>0.27200000000000002</v>
+        <v>0.27600000000000002</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="B29" s="3">
-        <v>4</v>
+        <v>3.9</v>
       </c>
       <c r="C29" s="3">
-        <v>9.6</v>
+        <v>9.5</v>
       </c>
       <c r="D29" s="3">
         <v>15.2</v>
       </c>
       <c r="E29" s="3">
-        <v>22.7</v>
+        <v>22.8</v>
       </c>
       <c r="F29" s="3">
-        <v>48.4</v>
+        <v>48.6</v>
       </c>
       <c r="G29" s="4">
-        <v>8.73</v>
+        <v>9.15</v>
       </c>
       <c r="H29" s="4">
-        <v>2.5099999999999998</v>
+        <v>2.56</v>
       </c>
       <c r="I29" s="4">
-        <v>3.48</v>
+        <v>3.58</v>
       </c>
       <c r="J29" s="5">
-        <v>0.443</v>
+        <v>0.44500000000000001</v>
       </c>
       <c r="K29" s="5">
-        <v>0.52300000000000002</v>
+        <v>0.54800000000000004</v>
       </c>
       <c r="L29" s="5">
         <v>0.373</v>
       </c>
       <c r="M29" s="5">
-        <v>8.8999999999999996E-2</v>
+        <v>0.09</v>
       </c>
       <c r="N29" s="5">
-        <v>0.17399999999999999</v>
+        <v>0.17599999999999999</v>
       </c>
       <c r="O29" s="5">
-        <v>0.26700000000000002</v>
+        <v>0.27200000000000002</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="B30" s="3">
         <v>4</v>
@@ -2957,183 +2957,183 @@
         <v>15.2</v>
       </c>
       <c r="E30" s="3">
-        <v>22.4</v>
+        <v>22.7</v>
       </c>
       <c r="F30" s="3">
-        <v>48.8</v>
+        <v>48.4</v>
       </c>
       <c r="G30" s="4">
-        <v>8.6300000000000008</v>
+        <v>8.73</v>
       </c>
       <c r="H30" s="4">
-        <v>2.5</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="I30" s="4">
-        <v>3.45</v>
+        <v>3.48</v>
       </c>
       <c r="J30" s="5">
-        <v>0.44600000000000001</v>
+        <v>0.443</v>
       </c>
       <c r="K30" s="5">
-        <v>0.52700000000000002</v>
+        <v>0.52300000000000002</v>
       </c>
       <c r="L30" s="5">
-        <v>0.38600000000000001</v>
+        <v>0.373</v>
       </c>
       <c r="M30" s="5">
-        <v>9.0999999999999998E-2</v>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="N30" s="5">
-        <v>0.17699999999999999</v>
+        <v>0.17399999999999999</v>
       </c>
       <c r="O30" s="5">
-        <v>0.27</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>29</v>
+        <v>0.26700000000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>2001</v>
       </c>
       <c r="B31" s="3">
-        <v>4.0999999999999996</v>
+        <v>4</v>
       </c>
       <c r="C31" s="3">
-        <v>9.8000000000000007</v>
+        <v>9.6</v>
       </c>
       <c r="D31" s="3">
         <v>15.2</v>
       </c>
       <c r="E31" s="3">
-        <v>22.3</v>
+        <v>22.4</v>
       </c>
       <c r="F31" s="3">
-        <v>48.6</v>
+        <v>48.8</v>
       </c>
       <c r="G31" s="4">
-        <v>8.58</v>
+        <v>8.6300000000000008</v>
       </c>
       <c r="H31" s="4">
         <v>2.5</v>
       </c>
       <c r="I31" s="4">
-        <v>3.44</v>
+        <v>3.45</v>
       </c>
       <c r="J31" s="5">
-        <v>0.442</v>
+        <v>0.44600000000000001</v>
       </c>
       <c r="K31" s="5">
-        <v>0.501</v>
+        <v>0.52700000000000002</v>
       </c>
       <c r="L31" s="5">
-        <v>0.38</v>
+        <v>0.38600000000000001</v>
       </c>
       <c r="M31" s="5">
-        <v>0.09</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="N31" s="5">
-        <v>0.17399999999999999</v>
+        <v>0.17699999999999999</v>
       </c>
       <c r="O31" s="5">
-        <v>0.26300000000000001</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" s="3">
-        <v>4</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="C32" s="3">
-        <v>9.6999999999999993</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="D32" s="3">
-        <v>15.3</v>
+        <v>15.2</v>
       </c>
       <c r="E32" s="3">
-        <v>22.6</v>
+        <v>22.3</v>
       </c>
       <c r="F32" s="3">
-        <v>48.4</v>
+        <v>48.6</v>
       </c>
       <c r="G32" s="4">
-        <v>8.7200000000000006</v>
+        <v>8.58</v>
       </c>
       <c r="H32" s="4">
         <v>2.5</v>
       </c>
       <c r="I32" s="4">
-        <v>3.49</v>
+        <v>3.44</v>
       </c>
       <c r="J32" s="5">
-        <v>0.441</v>
+        <v>0.442</v>
       </c>
       <c r="K32" s="5">
-        <v>0.49199999999999999</v>
+        <v>0.501</v>
       </c>
       <c r="L32" s="5">
-        <v>0.36599999999999999</v>
+        <v>0.38</v>
       </c>
       <c r="M32" s="5">
-        <v>8.7999999999999995E-2</v>
+        <v>0.09</v>
       </c>
       <c r="N32" s="5">
-        <v>0.17100000000000001</v>
+        <v>0.17399999999999999</v>
       </c>
       <c r="O32" s="5">
-        <v>0.26</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
-        <v>1998</v>
+        <v>0.26300000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="B33" s="3">
         <v>4</v>
       </c>
       <c r="C33" s="3">
-        <v>9.8000000000000007</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="D33" s="3">
-        <v>15.4</v>
+        <v>15.3</v>
       </c>
       <c r="E33" s="3">
-        <v>22.7</v>
+        <v>22.6</v>
       </c>
       <c r="F33" s="3">
-        <v>48.1</v>
+        <v>48.4</v>
       </c>
       <c r="G33" s="4">
         <v>8.7200000000000006</v>
       </c>
       <c r="H33" s="4">
-        <v>2.44</v>
+        <v>2.5</v>
       </c>
       <c r="I33" s="4">
-        <v>3.57</v>
+        <v>3.49</v>
       </c>
       <c r="J33" s="5">
-        <v>0.439</v>
+        <v>0.441</v>
       </c>
       <c r="K33" s="5">
-        <v>0.50600000000000001</v>
+        <v>0.49199999999999999</v>
       </c>
       <c r="L33" s="5">
-        <v>0.36899999999999999</v>
+        <v>0.36599999999999999</v>
       </c>
       <c r="M33" s="5">
         <v>8.7999999999999995E-2</v>
       </c>
       <c r="N33" s="5">
-        <v>0.17199999999999999</v>
+        <v>0.17100000000000001</v>
       </c>
       <c r="O33" s="5">
-        <v>0.26200000000000001</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="B34" s="3">
         <v>4</v>
@@ -3145,42 +3145,42 @@
         <v>15.4</v>
       </c>
       <c r="E34" s="3">
-        <v>22.6</v>
+        <v>22.7</v>
       </c>
       <c r="F34" s="3">
-        <v>48.3</v>
+        <v>48.1</v>
       </c>
       <c r="G34" s="4">
-        <v>8.93</v>
+        <v>8.7200000000000006</v>
       </c>
       <c r="H34" s="4">
-        <v>2.4700000000000002</v>
+        <v>2.44</v>
       </c>
       <c r="I34" s="4">
-        <v>3.61</v>
+        <v>3.57</v>
       </c>
       <c r="J34" s="5">
-        <v>0.44</v>
+        <v>0.439</v>
       </c>
       <c r="K34" s="5">
-        <v>0.5</v>
+        <v>0.50600000000000001</v>
       </c>
       <c r="L34" s="5">
-        <v>0.374</v>
+        <v>0.36899999999999999</v>
       </c>
       <c r="M34" s="5">
-        <v>8.8999999999999996E-2</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="N34" s="5">
-        <v>0.17299999999999999</v>
+        <v>0.17199999999999999</v>
       </c>
       <c r="O34" s="5">
-        <v>0.26300000000000001</v>
+        <v>0.26200000000000001</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <v>1996</v>
+        <v>1997</v>
       </c>
       <c r="B35" s="3">
         <v>4</v>
@@ -3189,98 +3189,98 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="D35" s="3">
+        <v>15.4</v>
+      </c>
+      <c r="E35" s="3">
+        <v>22.6</v>
+      </c>
+      <c r="F35" s="3">
+        <v>48.3</v>
+      </c>
+      <c r="G35" s="4">
+        <v>8.93</v>
+      </c>
+      <c r="H35" s="4">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="I35" s="4">
+        <v>3.61</v>
+      </c>
+      <c r="J35" s="5">
+        <v>0.44</v>
+      </c>
+      <c r="K35" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="L35" s="5">
+        <v>0.374</v>
+      </c>
+      <c r="M35" s="5">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="N35" s="5">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="O35" s="5">
+        <v>0.26300000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>1996</v>
+      </c>
+      <c r="B36" s="3">
+        <v>4</v>
+      </c>
+      <c r="C36" s="3">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="D36" s="3">
         <v>15.5</v>
       </c>
-      <c r="E35" s="3">
+      <c r="E36" s="3">
         <v>22.7</v>
       </c>
-      <c r="F35" s="3">
+      <c r="F36" s="3">
         <v>47.9</v>
       </c>
-      <c r="G35" s="4">
+      <c r="G36" s="4">
         <v>8.76</v>
       </c>
-      <c r="H35" s="4">
+      <c r="H36" s="4">
         <v>2.4500000000000002</v>
       </c>
-      <c r="I35" s="4">
+      <c r="I36" s="4">
         <v>3.57</v>
       </c>
-      <c r="J35" s="5">
+      <c r="J36" s="5">
         <v>0.437</v>
       </c>
-      <c r="K35" s="5">
+      <c r="K36" s="5">
         <v>0.47399999999999998</v>
       </c>
-      <c r="L35" s="5">
+      <c r="L36" s="5">
         <v>0.37</v>
       </c>
-      <c r="M35" s="5">
+      <c r="M36" s="5">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="N35" s="5">
+      <c r="N36" s="5">
         <v>0.17</v>
       </c>
-      <c r="O35" s="5">
+      <c r="O36" s="5">
         <v>0.25600000000000001</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B36" s="3">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="C36" s="3">
-        <v>9.9</v>
-      </c>
-      <c r="D36" s="3">
-        <v>15.6</v>
-      </c>
-      <c r="E36" s="3">
-        <v>22.8</v>
-      </c>
-      <c r="F36" s="3">
-        <v>47.6</v>
-      </c>
-      <c r="G36" s="4">
-        <v>8.59</v>
-      </c>
-      <c r="H36" s="4">
-        <v>2.42</v>
-      </c>
-      <c r="I36" s="4">
-        <v>3.55</v>
-      </c>
-      <c r="J36" s="5">
-        <v>0.433</v>
-      </c>
-      <c r="K36" s="5">
-        <v>0.46300000000000002</v>
-      </c>
-      <c r="L36" s="5">
-        <v>0.35599999999999998</v>
-      </c>
-      <c r="M36" s="5">
-        <v>8.5000000000000006E-2</v>
-      </c>
-      <c r="N36" s="5">
-        <v>0.16600000000000001</v>
-      </c>
-      <c r="O36" s="5">
-        <v>0.251</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B37" s="3">
-        <v>4</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="C37" s="3">
-        <v>9.8000000000000007</v>
+        <v>9.9</v>
       </c>
       <c r="D37" s="3">
         <v>15.6</v>
@@ -3289,42 +3289,42 @@
         <v>22.8</v>
       </c>
       <c r="F37" s="3">
-        <v>47.8</v>
+        <v>47.6</v>
       </c>
       <c r="G37" s="4">
-        <v>8.9499999999999993</v>
+        <v>8.59</v>
       </c>
       <c r="H37" s="4">
-        <v>2.4300000000000002</v>
+        <v>2.42</v>
       </c>
       <c r="I37" s="4">
-        <v>3.68</v>
+        <v>3.55</v>
       </c>
       <c r="J37" s="5">
-        <v>0.436</v>
+        <v>0.433</v>
       </c>
       <c r="K37" s="5">
-        <v>0.47399999999999998</v>
+        <v>0.46300000000000002</v>
       </c>
       <c r="L37" s="5">
-        <v>0.36299999999999999</v>
+        <v>0.35599999999999998</v>
       </c>
       <c r="M37" s="5">
-        <v>8.6999999999999994E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="N37" s="5">
-        <v>0.16900000000000001</v>
+        <v>0.16600000000000001</v>
       </c>
       <c r="O37" s="5">
-        <v>0.25600000000000001</v>
+        <v>0.251</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B38" s="3">
-        <v>3.9</v>
+        <v>4</v>
       </c>
       <c r="C38" s="3">
         <v>9.8000000000000007</v>
@@ -3333,25 +3333,25 @@
         <v>15.6</v>
       </c>
       <c r="E38" s="3">
-        <v>23</v>
+        <v>22.8</v>
       </c>
       <c r="F38" s="3">
-        <v>47.7</v>
+        <v>47.8</v>
       </c>
       <c r="G38" s="4">
-        <v>9.08</v>
+        <v>8.9499999999999993</v>
       </c>
       <c r="H38" s="4">
         <v>2.4300000000000002</v>
       </c>
       <c r="I38" s="4">
-        <v>3.73</v>
+        <v>3.68</v>
       </c>
       <c r="J38" s="5">
         <v>0.436</v>
       </c>
       <c r="K38" s="5">
-        <v>0.47199999999999998</v>
+        <v>0.47399999999999998</v>
       </c>
       <c r="L38" s="5">
         <v>0.36299999999999999</v>
@@ -3368,430 +3368,430 @@
     </row>
     <row r="39" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="C39" s="3">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="D39" s="3">
+        <v>15.6</v>
+      </c>
+      <c r="E39" s="3">
+        <v>23</v>
+      </c>
+      <c r="F39" s="3">
+        <v>47.7</v>
+      </c>
+      <c r="G39" s="4">
+        <v>9.08</v>
+      </c>
+      <c r="H39" s="4">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="I39" s="4">
+        <v>3.73</v>
+      </c>
+      <c r="J39" s="5">
+        <v>0.436</v>
+      </c>
+      <c r="K39" s="5">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="L39" s="5">
+        <v>0.36299999999999999</v>
+      </c>
+      <c r="M39" s="5">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="N39" s="5">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="O39" s="5">
+        <v>0.25600000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B40" s="3">
         <v>4.2</v>
       </c>
-      <c r="C39" s="3">
+      <c r="C40" s="3">
         <v>10.4</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D40" s="3">
         <v>16.3</v>
       </c>
-      <c r="E39" s="3">
+      <c r="E40" s="3">
         <v>23.7</v>
       </c>
-      <c r="F39" s="3">
+      <c r="F40" s="3">
         <v>45.5</v>
       </c>
-      <c r="G39" s="4">
+      <c r="G40" s="4">
         <v>8.6</v>
       </c>
-      <c r="H39" s="4">
+      <c r="H40" s="4">
         <v>2.34</v>
       </c>
-      <c r="I39" s="4">
+      <c r="I40" s="4">
         <v>3.68</v>
       </c>
-      <c r="J39" s="5">
+      <c r="J40" s="5">
         <v>0.41199999999999998</v>
       </c>
-      <c r="K39" s="5">
+      <c r="K40" s="5">
         <v>0.41599999999999998</v>
       </c>
-      <c r="L39" s="5">
+      <c r="L40" s="5">
         <v>0.29799999999999999</v>
       </c>
-      <c r="M39" s="5">
+      <c r="M40" s="5">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="N39" s="5">
+      <c r="N40" s="5">
         <v>0.14899999999999999</v>
       </c>
-      <c r="O39" s="5">
+      <c r="O40" s="5">
         <v>0.23</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" s="2">
-        <v>1991</v>
-      </c>
-      <c r="B40" s="3">
-        <v>4.3</v>
-      </c>
-      <c r="C40" s="3">
-        <v>10.6</v>
-      </c>
-      <c r="D40" s="3">
-        <v>16.5</v>
-      </c>
-      <c r="E40" s="3">
-        <v>23.6</v>
-      </c>
-      <c r="F40" s="3">
-        <v>45</v>
-      </c>
-      <c r="G40" s="4">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="H40" s="4">
-        <v>2.31</v>
-      </c>
-      <c r="I40" s="4">
-        <v>3.59</v>
-      </c>
-      <c r="J40" s="5">
-        <v>0.40600000000000003</v>
-      </c>
-      <c r="K40" s="5">
-        <v>0.39800000000000002</v>
-      </c>
-      <c r="L40" s="5">
-        <v>0.28899999999999998</v>
-      </c>
-      <c r="M40" s="5">
-        <v>7.0999999999999994E-2</v>
-      </c>
-      <c r="N40" s="5">
-        <v>0.14399999999999999</v>
-      </c>
-      <c r="O40" s="5">
-        <v>0.222</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <v>1990</v>
+        <v>1991</v>
       </c>
       <c r="B41" s="3">
-        <v>4.4000000000000004</v>
+        <v>4.3</v>
       </c>
       <c r="C41" s="3">
         <v>10.6</v>
       </c>
       <c r="D41" s="3">
-        <v>16.3</v>
+        <v>16.5</v>
       </c>
       <c r="E41" s="3">
-        <v>23.5</v>
+        <v>23.6</v>
       </c>
       <c r="F41" s="3">
-        <v>45.1</v>
+        <v>45</v>
       </c>
       <c r="G41" s="4">
-        <v>8.07</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="H41" s="4">
         <v>2.31</v>
       </c>
       <c r="I41" s="4">
-        <v>3.49</v>
+        <v>3.59</v>
       </c>
       <c r="J41" s="5">
         <v>0.40600000000000003</v>
       </c>
       <c r="K41" s="5">
-        <v>0.38600000000000001</v>
+        <v>0.39800000000000002</v>
       </c>
       <c r="L41" s="5">
-        <v>0.29199999999999998</v>
+        <v>0.28899999999999998</v>
       </c>
       <c r="M41" s="5">
-        <v>7.1999999999999995E-2</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="N41" s="5">
-        <v>0.14299999999999999</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="O41" s="5">
-        <v>0.22</v>
+        <v>0.222</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <v>1989</v>
+        <v>1990</v>
       </c>
       <c r="B42" s="3">
         <v>4.4000000000000004</v>
       </c>
       <c r="C42" s="3">
-        <v>10.5</v>
+        <v>10.6</v>
       </c>
       <c r="D42" s="3">
         <v>16.3</v>
       </c>
       <c r="E42" s="3">
-        <v>23.4</v>
+        <v>23.5</v>
       </c>
       <c r="F42" s="3">
-        <v>45.3</v>
+        <v>45.1</v>
       </c>
       <c r="G42" s="4">
-        <v>7.93</v>
+        <v>8.07</v>
       </c>
       <c r="H42" s="4">
         <v>2.31</v>
       </c>
       <c r="I42" s="4">
-        <v>3.43</v>
+        <v>3.49</v>
       </c>
       <c r="J42" s="5">
-        <v>0.40799999999999997</v>
+        <v>0.40600000000000003</v>
       </c>
       <c r="K42" s="5">
-        <v>0.39</v>
+        <v>0.38600000000000001</v>
       </c>
       <c r="L42" s="5">
-        <v>0.29699999999999999</v>
+        <v>0.29199999999999998</v>
       </c>
       <c r="M42" s="5">
-        <v>7.2999999999999995E-2</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="N42" s="5">
-        <v>0.14499999999999999</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="O42" s="5">
-        <v>0.222</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
-        <v>1988</v>
+        <v>1989</v>
       </c>
       <c r="B43" s="3">
         <v>4.4000000000000004</v>
       </c>
       <c r="C43" s="3">
-        <v>10.7</v>
+        <v>10.5</v>
       </c>
       <c r="D43" s="3">
-        <v>16.5</v>
+        <v>16.3</v>
       </c>
       <c r="E43" s="3">
-        <v>23.7</v>
+        <v>23.4</v>
       </c>
       <c r="F43" s="3">
-        <v>44.7</v>
+        <v>45.3</v>
       </c>
       <c r="G43" s="4">
-        <v>8.06</v>
+        <v>7.93</v>
       </c>
       <c r="H43" s="4">
-        <v>2.2799999999999998</v>
+        <v>2.31</v>
       </c>
       <c r="I43" s="4">
-        <v>3.53</v>
+        <v>3.43</v>
       </c>
       <c r="J43" s="5">
-        <v>0.40200000000000002</v>
+        <v>0.40799999999999997</v>
       </c>
       <c r="K43" s="5">
-        <v>0.379</v>
+        <v>0.39</v>
       </c>
       <c r="L43" s="5">
-        <v>0.28499999999999998</v>
+        <v>0.29699999999999999</v>
       </c>
       <c r="M43" s="5">
-        <v>7.0000000000000007E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="N43" s="5">
-        <v>0.14099999999999999</v>
+        <v>0.14499999999999999</v>
       </c>
       <c r="O43" s="5">
-        <v>0.216</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
-        <v>35</v>
+        <v>0.222</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>1988</v>
       </c>
       <c r="B44" s="3">
         <v>4.4000000000000004</v>
       </c>
       <c r="C44" s="3">
-        <v>10.8</v>
+        <v>10.7</v>
       </c>
       <c r="D44" s="3">
-        <v>16.7</v>
+        <v>16.5</v>
       </c>
       <c r="E44" s="3">
-        <v>23.8</v>
+        <v>23.7</v>
       </c>
       <c r="F44" s="3">
-        <v>44.4</v>
+        <v>44.7</v>
       </c>
       <c r="G44" s="4">
-        <v>8.07</v>
+        <v>8.06</v>
       </c>
       <c r="H44" s="4">
-        <v>2.25</v>
+        <v>2.2799999999999998</v>
       </c>
       <c r="I44" s="4">
-        <v>3.58</v>
+        <v>3.53</v>
       </c>
       <c r="J44" s="5">
-        <v>0.39900000000000002</v>
+        <v>0.40200000000000002</v>
       </c>
       <c r="K44" s="5">
         <v>0.379</v>
       </c>
       <c r="L44" s="5">
-        <v>0.28000000000000003</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="M44" s="5">
-        <v>6.9000000000000006E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="N44" s="5">
-        <v>0.13900000000000001</v>
+        <v>0.14099999999999999</v>
       </c>
       <c r="O44" s="5">
-        <v>0.215</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A45" s="2">
-        <v>1986</v>
+        <v>0.216</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="B45" s="3">
-        <v>4.5</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C45" s="3">
         <v>10.8</v>
       </c>
       <c r="D45" s="3">
-        <v>16.600000000000001</v>
+        <v>16.7</v>
       </c>
       <c r="E45" s="3">
         <v>23.8</v>
       </c>
       <c r="F45" s="3">
+        <v>44.4</v>
+      </c>
+      <c r="G45" s="4">
+        <v>8.07</v>
+      </c>
+      <c r="H45" s="4">
+        <v>2.25</v>
+      </c>
+      <c r="I45" s="4">
+        <v>3.58</v>
+      </c>
+      <c r="J45" s="5">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="K45" s="5">
+        <v>0.379</v>
+      </c>
+      <c r="L45" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="M45" s="5">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="N45" s="5">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="O45" s="5">
+        <v>0.215</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>1986</v>
+      </c>
+      <c r="B46" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="C46" s="3">
+        <v>10.8</v>
+      </c>
+      <c r="D46" s="3">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="E46" s="3">
+        <v>23.8</v>
+      </c>
+      <c r="F46" s="3">
         <v>44.3</v>
       </c>
-      <c r="G45" s="4">
+      <c r="G46" s="4">
         <v>7.8</v>
       </c>
-      <c r="H45" s="4">
+      <c r="H46" s="4">
         <v>2.27</v>
       </c>
-      <c r="I45" s="4">
+      <c r="I46" s="4">
         <v>3.44</v>
       </c>
-      <c r="J45" s="5">
+      <c r="J46" s="5">
         <v>0.39700000000000002</v>
       </c>
-      <c r="K45" s="5">
+      <c r="K46" s="5">
         <v>0.375</v>
       </c>
-      <c r="L45" s="5">
+      <c r="L46" s="5">
         <v>0.27600000000000002</v>
       </c>
-      <c r="M45" s="5">
+      <c r="M46" s="5">
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="N45" s="5">
+      <c r="N46" s="5">
         <v>0.13700000000000001</v>
       </c>
-      <c r="O45" s="5">
+      <c r="O46" s="5">
         <v>0.21199999999999999</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B46" s="3">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="C46" s="3">
-        <v>10.9</v>
-      </c>
-      <c r="D46" s="3">
-        <v>16.7</v>
-      </c>
-      <c r="E46" s="3">
-        <v>23.7</v>
-      </c>
-      <c r="F46" s="3">
-        <v>44.1</v>
-      </c>
-      <c r="G46" s="4">
-        <v>7.77</v>
-      </c>
-      <c r="H46" s="4">
-        <v>2.25</v>
-      </c>
-      <c r="I46" s="4">
-        <v>3.46</v>
-      </c>
-      <c r="J46" s="5">
-        <v>0.39400000000000002</v>
-      </c>
-      <c r="K46" s="5">
-        <v>0.36899999999999999</v>
-      </c>
-      <c r="L46" s="5">
-        <v>0.26900000000000002</v>
-      </c>
-      <c r="M46" s="5">
-        <v>6.7000000000000004E-2</v>
-      </c>
-      <c r="N46" s="5">
-        <v>0.13500000000000001</v>
-      </c>
-      <c r="O46" s="5">
-        <v>0.20799999999999999</v>
       </c>
     </row>
     <row r="47" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B47" s="3">
         <v>4.5999999999999996</v>
       </c>
       <c r="C47" s="3">
-        <v>11</v>
+        <v>10.9</v>
       </c>
       <c r="D47" s="3">
-        <v>16.8</v>
+        <v>16.7</v>
       </c>
       <c r="E47" s="3">
-        <v>24</v>
+        <v>23.7</v>
       </c>
       <c r="F47" s="3">
-        <v>43.6</v>
+        <v>44.1</v>
       </c>
       <c r="G47" s="4">
-        <v>7.81</v>
+        <v>7.77</v>
       </c>
       <c r="H47" s="4">
-        <v>2.23</v>
+        <v>2.25</v>
       </c>
       <c r="I47" s="4">
-        <v>3.5</v>
+        <v>3.46</v>
       </c>
       <c r="J47" s="5">
-        <v>0.38900000000000001</v>
+        <v>0.39400000000000002</v>
       </c>
       <c r="K47" s="5">
-        <v>0.36599999999999999</v>
+        <v>0.36899999999999999</v>
       </c>
       <c r="L47" s="5">
-        <v>0.26100000000000001</v>
+        <v>0.26900000000000002</v>
       </c>
       <c r="M47" s="5">
-        <v>6.5000000000000002E-2</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="N47" s="5">
-        <v>0.13200000000000001</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="O47" s="5">
-        <v>0.20499999999999999</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
-        <v>1983</v>
+        <v>0.20799999999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="B48" s="3">
         <v>4.5999999999999996</v>
@@ -3800,31 +3800,31 @@
         <v>11</v>
       </c>
       <c r="D48" s="3">
-        <v>16.899999999999999</v>
+        <v>16.8</v>
       </c>
       <c r="E48" s="3">
         <v>24</v>
       </c>
       <c r="F48" s="3">
-        <v>43.5</v>
+        <v>43.6</v>
       </c>
       <c r="G48" s="4">
-        <v>7.52</v>
+        <v>7.81</v>
       </c>
       <c r="H48" s="4">
-        <v>2.21</v>
+        <v>2.23</v>
       </c>
       <c r="I48" s="4">
-        <v>3.41</v>
+        <v>3.5</v>
       </c>
       <c r="J48" s="5">
         <v>0.38900000000000001</v>
       </c>
       <c r="K48" s="5">
-        <v>0.373</v>
+        <v>0.36599999999999999</v>
       </c>
       <c r="L48" s="5">
-        <v>0.26</v>
+        <v>0.26100000000000001</v>
       </c>
       <c r="M48" s="5">
         <v>6.5000000000000002E-2</v>
@@ -3833,183 +3833,183 @@
         <v>0.13200000000000001</v>
       </c>
       <c r="O48" s="5">
-        <v>0.20699999999999999</v>
+        <v>0.20499999999999999</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
-        <v>1982</v>
+        <v>1983</v>
       </c>
       <c r="B49" s="3">
-        <v>4.7</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C49" s="3">
-        <v>11.1</v>
+        <v>11</v>
       </c>
       <c r="D49" s="3">
-        <v>17</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="E49" s="3">
-        <v>23.9</v>
+        <v>24</v>
       </c>
       <c r="F49" s="3">
-        <v>43.2</v>
+        <v>43.5</v>
       </c>
       <c r="G49" s="4">
-        <v>6.94</v>
+        <v>7.52</v>
       </c>
       <c r="H49" s="4">
-        <v>2.15</v>
+        <v>2.21</v>
       </c>
       <c r="I49" s="4">
-        <v>3.23</v>
+        <v>3.41</v>
       </c>
       <c r="J49" s="5">
-        <v>0.38400000000000001</v>
+        <v>0.38900000000000001</v>
       </c>
       <c r="K49" s="5">
-        <v>0.37</v>
+        <v>0.373</v>
       </c>
       <c r="L49" s="5">
-        <v>0.255</v>
+        <v>0.26</v>
       </c>
       <c r="M49" s="5">
-        <v>6.4000000000000001E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="N49" s="5">
-        <v>0.129</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="O49" s="5">
-        <v>0.20300000000000001</v>
+        <v>0.20699999999999999</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
-        <v>1981</v>
+        <v>1982</v>
       </c>
       <c r="B50" s="3">
-        <v>5</v>
+        <v>4.7</v>
       </c>
       <c r="C50" s="3">
-        <v>11.4</v>
+        <v>11.1</v>
       </c>
       <c r="D50" s="3">
-        <v>17.2</v>
+        <v>17</v>
       </c>
       <c r="E50" s="3">
-        <v>24</v>
+        <v>23.9</v>
       </c>
       <c r="F50" s="3">
-        <v>42.4</v>
+        <v>43.2</v>
       </c>
       <c r="G50" s="4">
-        <v>6.75</v>
+        <v>6.94</v>
       </c>
       <c r="H50" s="4">
-        <v>2.13</v>
+        <v>2.15</v>
       </c>
       <c r="I50" s="4">
-        <v>3.17</v>
+        <v>3.23</v>
       </c>
       <c r="J50" s="5">
-        <v>0.373</v>
+        <v>0.38400000000000001</v>
       </c>
       <c r="K50" s="5">
-        <v>0.34599999999999997</v>
+        <v>0.37</v>
       </c>
       <c r="L50" s="5">
-        <v>0.24</v>
+        <v>0.255</v>
       </c>
       <c r="M50" s="5">
-        <v>0.06</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="N50" s="5">
-        <v>0.122</v>
+        <v>0.129</v>
       </c>
       <c r="O50" s="5">
-        <v>0.192</v>
+        <v>0.20300000000000001</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
-        <v>1980</v>
+        <v>1981</v>
       </c>
       <c r="B51" s="3">
-        <v>5.2</v>
+        <v>5</v>
       </c>
       <c r="C51" s="3">
-        <v>11.6</v>
+        <v>11.4</v>
       </c>
       <c r="D51" s="3">
-        <v>17.3</v>
+        <v>17.2</v>
       </c>
       <c r="E51" s="3">
         <v>24</v>
       </c>
       <c r="F51" s="3">
-        <v>41.9</v>
+        <v>42.4</v>
       </c>
       <c r="G51" s="4">
-        <v>6.52</v>
+        <v>6.75</v>
       </c>
       <c r="H51" s="4">
-        <v>2.1</v>
+        <v>2.13</v>
       </c>
       <c r="I51" s="4">
-        <v>3.11</v>
+        <v>3.17</v>
       </c>
       <c r="J51" s="5">
-        <v>0.36699999999999999</v>
+        <v>0.373</v>
       </c>
       <c r="K51" s="5">
-        <v>0.32500000000000001</v>
+        <v>0.34599999999999997</v>
       </c>
       <c r="L51" s="5">
-        <v>0.23300000000000001</v>
+        <v>0.24</v>
       </c>
       <c r="M51" s="5">
-        <v>5.8000000000000003E-2</v>
+        <v>0.06</v>
       </c>
       <c r="N51" s="5">
-        <v>0.11799999999999999</v>
+        <v>0.122</v>
       </c>
       <c r="O51" s="5">
-        <v>0.184</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="6" t="s">
-        <v>38</v>
+        <v>0.192</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>1980</v>
       </c>
       <c r="B52" s="3">
-        <v>5.3</v>
+        <v>5.2</v>
       </c>
       <c r="C52" s="3">
-        <v>11.7</v>
+        <v>11.6</v>
       </c>
       <c r="D52" s="3">
-        <v>17.2</v>
+        <v>17.3</v>
       </c>
       <c r="E52" s="3">
-        <v>23.8</v>
+        <v>24</v>
       </c>
       <c r="F52" s="3">
         <v>41.9</v>
       </c>
       <c r="G52" s="4">
-        <v>6.33</v>
+        <v>6.52</v>
       </c>
       <c r="H52" s="4">
-        <v>2.09</v>
+        <v>2.1</v>
       </c>
       <c r="I52" s="4">
-        <v>3.03</v>
+        <v>3.11</v>
       </c>
       <c r="J52" s="5">
-        <v>0.36599999999999999</v>
+        <v>0.36699999999999999</v>
       </c>
       <c r="K52" s="5">
-        <v>0.314</v>
+        <v>0.32500000000000001</v>
       </c>
       <c r="L52" s="5">
         <v>0.23300000000000001</v>
@@ -4018,68 +4018,68 @@
         <v>5.8000000000000003E-2</v>
       </c>
       <c r="N52" s="5">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="O52" s="5">
+        <v>0.184</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B53" s="3">
+        <v>5.3</v>
+      </c>
+      <c r="C53" s="3">
+        <v>11.7</v>
+      </c>
+      <c r="D53" s="3">
+        <v>17.2</v>
+      </c>
+      <c r="E53" s="3">
+        <v>23.8</v>
+      </c>
+      <c r="F53" s="3">
+        <v>41.9</v>
+      </c>
+      <c r="G53" s="4">
+        <v>6.33</v>
+      </c>
+      <c r="H53" s="4">
+        <v>2.09</v>
+      </c>
+      <c r="I53" s="4">
+        <v>3.03</v>
+      </c>
+      <c r="J53" s="5">
+        <v>0.36599999999999999</v>
+      </c>
+      <c r="K53" s="5">
+        <v>0.314</v>
+      </c>
+      <c r="L53" s="5">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="M53" s="5">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="N53" s="5">
         <v>0.11700000000000001</v>
       </c>
-      <c r="O52" s="5">
+      <c r="O53" s="5">
         <v>0.182</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A53" s="2">
-        <v>1978</v>
-      </c>
-      <c r="B53" s="3">
-        <v>5.4</v>
-      </c>
-      <c r="C53" s="3">
-        <v>11.8</v>
-      </c>
-      <c r="D53" s="3">
-        <v>17.3</v>
-      </c>
-      <c r="E53" s="3">
-        <v>23.7</v>
-      </c>
-      <c r="F53" s="3">
-        <v>41.8</v>
-      </c>
-      <c r="G53" s="4">
-        <v>6.2</v>
-      </c>
-      <c r="H53" s="4">
-        <v>2.08</v>
-      </c>
-      <c r="I53" s="4">
-        <v>2.98</v>
-      </c>
-      <c r="J53" s="5">
-        <v>0.36299999999999999</v>
-      </c>
-      <c r="K53" s="5">
-        <v>0.308</v>
-      </c>
-      <c r="L53" s="5">
-        <v>0.23</v>
-      </c>
-      <c r="M53" s="5">
-        <v>5.7000000000000002E-2</v>
-      </c>
-      <c r="N53" s="5">
-        <v>0.115</v>
-      </c>
-      <c r="O53" s="5">
-        <v>0.17799999999999999</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
-        <v>1977</v>
+        <v>1978</v>
       </c>
       <c r="B54" s="3">
-        <v>5.5</v>
+        <v>5.4</v>
       </c>
       <c r="C54" s="3">
-        <v>11.7</v>
+        <v>11.8</v>
       </c>
       <c r="D54" s="3">
         <v>17.3</v>
@@ -4088,22 +4088,22 @@
         <v>23.7</v>
       </c>
       <c r="F54" s="3">
-        <v>41.7</v>
+        <v>41.8</v>
       </c>
       <c r="G54" s="4">
-        <v>6.06</v>
+        <v>6.2</v>
       </c>
       <c r="H54" s="4">
-        <v>2.06</v>
+        <v>2.08</v>
       </c>
       <c r="I54" s="4">
-        <v>2.95</v>
+        <v>2.98</v>
       </c>
       <c r="J54" s="5">
-        <v>0.36199999999999999</v>
+        <v>0.36299999999999999</v>
       </c>
       <c r="K54" s="5">
-        <v>0.309</v>
+        <v>0.308</v>
       </c>
       <c r="L54" s="5">
         <v>0.23</v>
@@ -4118,95 +4118,95 @@
         <v>0.17799999999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="6" t="s">
-        <v>39</v>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <v>1977</v>
       </c>
       <c r="B55" s="3">
-        <v>5.6</v>
+        <v>5.5</v>
       </c>
       <c r="C55" s="3">
-        <v>11.8</v>
+        <v>11.7</v>
       </c>
       <c r="D55" s="3">
-        <v>17.399999999999999</v>
+        <v>17.3</v>
       </c>
       <c r="E55" s="3">
-        <v>23.8</v>
+        <v>23.7</v>
       </c>
       <c r="F55" s="3">
-        <v>41.5</v>
+        <v>41.7</v>
       </c>
       <c r="G55" s="4">
-        <v>6.07</v>
+        <v>6.06</v>
       </c>
       <c r="H55" s="4">
         <v>2.06</v>
       </c>
       <c r="I55" s="4">
-        <v>2.94</v>
+        <v>2.95</v>
       </c>
       <c r="J55" s="5">
-        <v>0.35899999999999999</v>
+        <v>0.36199999999999999</v>
       </c>
       <c r="K55" s="5">
-        <v>0.30099999999999999</v>
+        <v>0.309</v>
       </c>
       <c r="L55" s="5">
-        <v>0.22500000000000001</v>
+        <v>0.23</v>
       </c>
       <c r="M55" s="5">
-        <v>5.6000000000000001E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="N55" s="5">
-        <v>0.112</v>
+        <v>0.115</v>
       </c>
       <c r="O55" s="5">
-        <v>0.17399999999999999</v>
+        <v>0.17799999999999999</v>
       </c>
     </row>
     <row r="56" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B56" s="3">
         <v>5.6</v>
       </c>
       <c r="C56" s="3">
-        <v>11.9</v>
+        <v>11.8</v>
       </c>
       <c r="D56" s="3">
-        <v>17.3</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="E56" s="3">
-        <v>23.6</v>
+        <v>23.8</v>
       </c>
       <c r="F56" s="3">
-        <v>41.6</v>
+        <v>41.5</v>
       </c>
       <c r="G56" s="4">
-        <v>5.86</v>
+        <v>6.07</v>
       </c>
       <c r="H56" s="4">
-        <v>2.0499999999999998</v>
+        <v>2.06</v>
       </c>
       <c r="I56" s="4">
-        <v>2.86</v>
+        <v>2.94</v>
       </c>
       <c r="J56" s="5">
         <v>0.35899999999999999</v>
       </c>
       <c r="K56" s="5">
-        <v>0.29799999999999999</v>
+        <v>0.30099999999999999</v>
       </c>
       <c r="L56" s="5">
-        <v>0.22600000000000001</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="M56" s="5">
         <v>5.6000000000000001E-2</v>
       </c>
       <c r="N56" s="5">
-        <v>0.113</v>
+        <v>0.112</v>
       </c>
       <c r="O56" s="5">
         <v>0.17399999999999999</v>
@@ -4214,13 +4214,13 @@
     </row>
     <row r="57" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B57" s="3">
-        <v>5.8</v>
+        <v>5.6</v>
       </c>
       <c r="C57" s="3">
-        <v>12.1</v>
+        <v>11.9</v>
       </c>
       <c r="D57" s="3">
         <v>17.3</v>
@@ -4229,139 +4229,139 @@
         <v>23.6</v>
       </c>
       <c r="F57" s="3">
+        <v>41.6</v>
+      </c>
+      <c r="G57" s="4">
+        <v>5.86</v>
+      </c>
+      <c r="H57" s="4">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="I57" s="4">
+        <v>2.86</v>
+      </c>
+      <c r="J57" s="5">
+        <v>0.35899999999999999</v>
+      </c>
+      <c r="K57" s="5">
+        <v>0.29799999999999999</v>
+      </c>
+      <c r="L57" s="5">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="M57" s="5">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="N57" s="5">
+        <v>0.113</v>
+      </c>
+      <c r="O57" s="5">
+        <v>0.17399999999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B58" s="3">
+        <v>5.8</v>
+      </c>
+      <c r="C58" s="3">
+        <v>12.1</v>
+      </c>
+      <c r="D58" s="3">
+        <v>17.3</v>
+      </c>
+      <c r="E58" s="3">
+        <v>23.6</v>
+      </c>
+      <c r="F58" s="3">
         <v>41.2</v>
-      </c>
-      <c r="G57" s="4">
-        <v>6.11</v>
-      </c>
-      <c r="H57" s="4">
-        <v>2.09</v>
-      </c>
-      <c r="I57" s="4">
-        <v>2.92</v>
-      </c>
-      <c r="J57" s="5">
-        <v>0.35399999999999998</v>
-      </c>
-      <c r="K57" s="5">
-        <v>0.28799999999999998</v>
-      </c>
-      <c r="L57" s="5">
-        <v>0.22</v>
-      </c>
-      <c r="M57" s="5">
-        <v>5.5E-2</v>
-      </c>
-      <c r="N57" s="5">
-        <v>0.11</v>
-      </c>
-      <c r="O57" s="5">
-        <v>0.16900000000000001</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58" s="2">
-        <v>1973</v>
-      </c>
-      <c r="B58" s="3">
-        <v>5.6</v>
-      </c>
-      <c r="C58" s="3">
-        <v>12</v>
-      </c>
-      <c r="D58" s="3">
-        <v>17.2</v>
-      </c>
-      <c r="E58" s="3">
-        <v>23.5</v>
-      </c>
-      <c r="F58" s="3">
-        <v>41.7</v>
       </c>
       <c r="G58" s="4">
         <v>6.11</v>
       </c>
       <c r="H58" s="4">
-        <v>2.08</v>
+        <v>2.09</v>
       </c>
       <c r="I58" s="4">
-        <v>2.94</v>
+        <v>2.92</v>
       </c>
       <c r="J58" s="5">
-        <v>0.36</v>
+        <v>0.35399999999999998</v>
       </c>
       <c r="K58" s="5">
         <v>0.28799999999999998</v>
       </c>
       <c r="L58" s="5">
-        <v>0.22800000000000001</v>
+        <v>0.22</v>
       </c>
       <c r="M58" s="5">
-        <v>5.6000000000000001E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="N58" s="5">
-        <v>0.113</v>
+        <v>0.11</v>
       </c>
       <c r="O58" s="5">
-        <v>0.17299999999999999</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="6" t="s">
-        <v>42</v>
+        <v>0.16900000000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>1973</v>
       </c>
       <c r="B59" s="3">
         <v>5.6</v>
       </c>
       <c r="C59" s="3">
-        <v>11.9</v>
+        <v>12</v>
       </c>
       <c r="D59" s="3">
         <v>17.2</v>
       </c>
       <c r="E59" s="3">
-        <v>23.4</v>
+        <v>23.5</v>
       </c>
       <c r="F59" s="3">
-        <v>41.9</v>
+        <v>41.7</v>
       </c>
       <c r="G59" s="4">
-        <v>5.89</v>
+        <v>6.11</v>
       </c>
       <c r="H59" s="4">
-        <v>2.0699999999999998</v>
+        <v>2.08</v>
       </c>
       <c r="I59" s="4">
-        <v>2.85</v>
+        <v>2.94</v>
       </c>
       <c r="J59" s="5">
-        <v>0.36199999999999999</v>
+        <v>0.36</v>
       </c>
       <c r="K59" s="5">
-        <v>0.30099999999999999</v>
+        <v>0.28799999999999998</v>
       </c>
       <c r="L59" s="5">
-        <v>0.23300000000000001</v>
+        <v>0.22800000000000001</v>
       </c>
       <c r="M59" s="5">
-        <v>5.7000000000000002E-2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="N59" s="5">
-        <v>0.115</v>
+        <v>0.113</v>
       </c>
       <c r="O59" s="5">
-        <v>0.17699999999999999</v>
+        <v>0.17299999999999999</v>
       </c>
     </row>
     <row r="60" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B60" s="3">
-        <v>5.7</v>
+        <v>5.6</v>
       </c>
       <c r="C60" s="3">
-        <v>12</v>
+        <v>11.9</v>
       </c>
       <c r="D60" s="3">
         <v>17.2</v>
@@ -4370,78 +4370,78 @@
         <v>23.4</v>
       </c>
       <c r="F60" s="3">
-        <v>41.7</v>
+        <v>41.9</v>
       </c>
       <c r="G60" s="4">
-        <v>5.86</v>
+        <v>5.89</v>
       </c>
       <c r="H60" s="4">
-        <v>2.0499999999999998</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="I60" s="4">
-        <v>2.86</v>
+        <v>2.85</v>
       </c>
       <c r="J60" s="5">
-        <v>0.35899999999999999</v>
+        <v>0.36199999999999999</v>
       </c>
       <c r="K60" s="5">
-        <v>0.29699999999999999</v>
+        <v>0.30099999999999999</v>
       </c>
       <c r="L60" s="5">
-        <v>0.22900000000000001</v>
+        <v>0.23300000000000001</v>
       </c>
       <c r="M60" s="5">
-        <v>5.6000000000000001E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="N60" s="5">
-        <v>0.113</v>
+        <v>0.115</v>
       </c>
       <c r="O60" s="5">
-        <v>0.17399999999999999</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" s="2">
-        <v>1970</v>
+        <v>0.17699999999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="B61" s="3">
         <v>5.7</v>
       </c>
       <c r="C61" s="3">
-        <v>12.1</v>
+        <v>12</v>
       </c>
       <c r="D61" s="3">
-        <v>17.3</v>
+        <v>17.2</v>
       </c>
       <c r="E61" s="3">
         <v>23.4</v>
       </c>
       <c r="F61" s="3">
-        <v>41.5</v>
+        <v>41.7</v>
       </c>
       <c r="G61" s="4">
-        <v>5.76</v>
+        <v>5.86</v>
       </c>
       <c r="H61" s="4">
-        <v>2.0299999999999998</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="I61" s="4">
-        <v>2.84</v>
+        <v>2.86</v>
       </c>
       <c r="J61" s="5">
-        <v>0.35699999999999998</v>
+        <v>0.35899999999999999</v>
       </c>
       <c r="K61" s="5">
         <v>0.29699999999999999</v>
       </c>
       <c r="L61" s="5">
-        <v>0.22700000000000001</v>
+        <v>0.22900000000000001</v>
       </c>
       <c r="M61" s="5">
         <v>5.6000000000000001E-2</v>
       </c>
       <c r="N61" s="5">
-        <v>0.112</v>
+        <v>0.113</v>
       </c>
       <c r="O61" s="5">
         <v>0.17399999999999999</v>
@@ -4449,13 +4449,13 @@
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
-        <v>1969</v>
+        <v>1970</v>
       </c>
       <c r="B62" s="3">
-        <v>5.8</v>
+        <v>5.7</v>
       </c>
       <c r="C62" s="3">
-        <v>12.2</v>
+        <v>12.1</v>
       </c>
       <c r="D62" s="3">
         <v>17.3</v>
@@ -4464,75 +4464,75 @@
         <v>23.4</v>
       </c>
       <c r="F62" s="3">
-        <v>41.3</v>
+        <v>41.5</v>
       </c>
       <c r="G62" s="4">
-        <v>5.7</v>
+        <v>5.76</v>
       </c>
       <c r="H62" s="4">
-        <v>2.02</v>
+        <v>2.0299999999999998</v>
       </c>
       <c r="I62" s="4">
-        <v>2.83</v>
+        <v>2.84</v>
       </c>
       <c r="J62" s="5">
-        <v>0.35299999999999998</v>
+        <v>0.35699999999999998</v>
       </c>
       <c r="K62" s="5">
-        <v>0.28100000000000003</v>
+        <v>0.29699999999999999</v>
       </c>
       <c r="L62" s="5">
-        <v>0.223</v>
+        <v>0.22700000000000001</v>
       </c>
       <c r="M62" s="5">
-        <v>5.5E-2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="N62" s="5">
-        <v>0.109</v>
+        <v>0.112</v>
       </c>
       <c r="O62" s="5">
-        <v>0.16800000000000001</v>
+        <v>0.17399999999999999</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
-        <v>1968</v>
+        <v>1969</v>
       </c>
       <c r="B63" s="3">
         <v>5.8</v>
       </c>
       <c r="C63" s="3">
-        <v>12.3</v>
+        <v>12.2</v>
       </c>
       <c r="D63" s="3">
-        <v>17.399999999999999</v>
+        <v>17.3</v>
       </c>
       <c r="E63" s="3">
         <v>23.4</v>
       </c>
       <c r="F63" s="3">
-        <v>41.1</v>
+        <v>41.3</v>
       </c>
       <c r="G63" s="4">
-        <v>5.94</v>
+        <v>5.7</v>
       </c>
       <c r="H63" s="4">
-        <v>2.0699999999999998</v>
+        <v>2.02</v>
       </c>
       <c r="I63" s="4">
-        <v>2.87</v>
+        <v>2.83</v>
       </c>
       <c r="J63" s="5">
-        <v>0.35099999999999998</v>
+        <v>0.35299999999999998</v>
       </c>
       <c r="K63" s="5">
-        <v>0.28399999999999997</v>
+        <v>0.28100000000000003</v>
       </c>
       <c r="L63" s="5">
-        <v>0.22</v>
+        <v>0.223</v>
       </c>
       <c r="M63" s="5">
-        <v>5.3999999999999999E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="N63" s="5">
         <v>0.109</v>
@@ -4541,75 +4541,103 @@
         <v>0.16800000000000001</v>
       </c>
     </row>
-    <row r="64" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="6" t="s">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>1968</v>
+      </c>
+      <c r="B64" s="3">
+        <v>5.8</v>
+      </c>
+      <c r="C64" s="3">
+        <v>12.3</v>
+      </c>
+      <c r="D64" s="3">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="E64" s="3">
+        <v>23.4</v>
+      </c>
+      <c r="F64" s="3">
+        <v>41.1</v>
+      </c>
+      <c r="G64" s="4">
+        <v>5.94</v>
+      </c>
+      <c r="H64" s="4">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="I64" s="4">
+        <v>2.87</v>
+      </c>
+      <c r="J64" s="5">
+        <v>0.35099999999999998</v>
+      </c>
+      <c r="K64" s="5">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="L64" s="5">
+        <v>0.22</v>
+      </c>
+      <c r="M64" s="5">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="N64" s="5">
+        <v>0.109</v>
+      </c>
+      <c r="O64" s="5">
+        <v>0.16800000000000001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B64" s="3">
+      <c r="B65" s="3">
         <v>5.6</v>
       </c>
-      <c r="C64" s="3">
+      <c r="C65" s="3">
         <v>12</v>
       </c>
-      <c r="D64" s="3">
+      <c r="D65" s="3">
         <v>17.100000000000001</v>
       </c>
-      <c r="E64" s="3">
+      <c r="E65" s="3">
         <v>23.2</v>
       </c>
-      <c r="F64" s="3">
+      <c r="F65" s="3">
         <v>42.1</v>
       </c>
-      <c r="G64" s="4">
+      <c r="G65" s="4">
         <v>5.84</v>
       </c>
-      <c r="H64" s="4">
+      <c r="H65" s="4">
         <v>2.0499999999999998</v>
       </c>
-      <c r="I64" s="4">
+      <c r="I65" s="4">
         <v>2.84</v>
       </c>
-      <c r="J64" s="5">
+      <c r="J65" s="5">
         <v>0.36199999999999999</v>
       </c>
-      <c r="K64" s="5">
+      <c r="K65" s="5">
         <v>0.30199999999999999</v>
       </c>
-      <c r="L64" s="5">
+      <c r="L65" s="5">
         <v>0.23799999999999999</v>
       </c>
-      <c r="M64" s="5">
+      <c r="M65" s="5">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="N64" s="5">
+      <c r="N65" s="5">
         <v>0.11600000000000001</v>
       </c>
-      <c r="O64" s="5">
+      <c r="O65" s="5">
         <v>0.17799999999999999</v>
       </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A65" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B65" s="11"/>
-      <c r="C65" s="11"/>
-      <c r="D65" s="11"/>
-      <c r="E65" s="11"/>
-      <c r="F65" s="11"/>
-      <c r="G65" s="11"/>
-      <c r="H65" s="11"/>
-      <c r="I65" s="11"/>
-      <c r="J65" s="11"/>
-      <c r="K65" s="11"/>
-      <c r="L65" s="11"/>
-      <c r="M65" s="11"/>
-      <c r="N65" s="11"/>
-      <c r="O65" s="11"/>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B66" s="11"/>
       <c r="C66" s="11"/>
@@ -4627,46 +4655,46 @@
       <c r="O66" s="11"/>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A67" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B67" s="9"/>
-      <c r="C67" s="9"/>
-      <c r="D67" s="9"/>
-      <c r="E67" s="9"/>
-      <c r="F67" s="9"/>
-      <c r="G67" s="9"/>
-      <c r="H67" s="9"/>
-      <c r="I67" s="9"/>
-      <c r="J67" s="9"/>
-      <c r="K67" s="9"/>
-      <c r="L67" s="9"/>
-      <c r="M67" s="9"/>
-      <c r="N67" s="9"/>
-      <c r="O67" s="9"/>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A68" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B68" s="11"/>
-      <c r="C68" s="11"/>
-      <c r="D68" s="11"/>
-      <c r="E68" s="11"/>
-      <c r="F68" s="11"/>
-      <c r="G68" s="11"/>
-      <c r="H68" s="11"/>
-      <c r="I68" s="11"/>
-      <c r="J68" s="11"/>
-      <c r="K68" s="11"/>
-      <c r="L68" s="11"/>
-      <c r="M68" s="11"/>
-      <c r="N68" s="11"/>
-      <c r="O68" s="11"/>
+      <c r="A67" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B67" s="11"/>
+      <c r="C67" s="11"/>
+      <c r="D67" s="11"/>
+      <c r="E67" s="11"/>
+      <c r="F67" s="11"/>
+      <c r="G67" s="11"/>
+      <c r="H67" s="11"/>
+      <c r="I67" s="11"/>
+      <c r="J67" s="11"/>
+      <c r="K67" s="11"/>
+      <c r="L67" s="11"/>
+      <c r="M67" s="11"/>
+      <c r="N67" s="11"/>
+      <c r="O67" s="11"/>
+    </row>
+    <row r="68" spans="1:15" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B68" s="9"/>
+      <c r="C68" s="9"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="9"/>
+      <c r="G68" s="9"/>
+      <c r="H68" s="9"/>
+      <c r="I68" s="9"/>
+      <c r="J68" s="9"/>
+      <c r="K68" s="9"/>
+      <c r="L68" s="9"/>
+      <c r="M68" s="9"/>
+      <c r="N68" s="9"/>
+      <c r="O68" s="9"/>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B69" s="11"/>
       <c r="C69" s="11"/>
@@ -4685,7 +4713,7 @@
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="11" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="B70" s="11"/>
       <c r="C70" s="11"/>
@@ -4704,7 +4732,7 @@
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B71" s="11"/>
       <c r="C71" s="11"/>
@@ -4723,7 +4751,7 @@
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B72" s="11"/>
       <c r="C72" s="11"/>
@@ -4742,7 +4770,7 @@
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B73" s="11"/>
       <c r="C73" s="11"/>
@@ -4761,7 +4789,7 @@
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B74" s="11"/>
       <c r="C74" s="11"/>
@@ -4779,46 +4807,46 @@
       <c r="O74" s="11"/>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A75" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B75" s="9"/>
-      <c r="C75" s="9"/>
-      <c r="D75" s="9"/>
-      <c r="E75" s="9"/>
-      <c r="F75" s="9"/>
-      <c r="G75" s="9"/>
-      <c r="H75" s="9"/>
-      <c r="I75" s="9"/>
-      <c r="J75" s="9"/>
-      <c r="K75" s="9"/>
-      <c r="L75" s="9"/>
-      <c r="M75" s="9"/>
-      <c r="N75" s="9"/>
-      <c r="O75" s="9"/>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A76" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B76" s="11"/>
-      <c r="C76" s="11"/>
-      <c r="D76" s="11"/>
-      <c r="E76" s="11"/>
-      <c r="F76" s="11"/>
-      <c r="G76" s="11"/>
-      <c r="H76" s="11"/>
-      <c r="I76" s="11"/>
-      <c r="J76" s="11"/>
-      <c r="K76" s="11"/>
-      <c r="L76" s="11"/>
-      <c r="M76" s="11"/>
-      <c r="N76" s="11"/>
-      <c r="O76" s="11"/>
+      <c r="A75" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B75" s="11"/>
+      <c r="C75" s="11"/>
+      <c r="D75" s="11"/>
+      <c r="E75" s="11"/>
+      <c r="F75" s="11"/>
+      <c r="G75" s="11"/>
+      <c r="H75" s="11"/>
+      <c r="I75" s="11"/>
+      <c r="J75" s="11"/>
+      <c r="K75" s="11"/>
+      <c r="L75" s="11"/>
+      <c r="M75" s="11"/>
+      <c r="N75" s="11"/>
+      <c r="O75" s="11"/>
+    </row>
+    <row r="76" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B76" s="9"/>
+      <c r="C76" s="9"/>
+      <c r="D76" s="9"/>
+      <c r="E76" s="9"/>
+      <c r="F76" s="9"/>
+      <c r="G76" s="9"/>
+      <c r="H76" s="9"/>
+      <c r="I76" s="9"/>
+      <c r="J76" s="9"/>
+      <c r="K76" s="9"/>
+      <c r="L76" s="9"/>
+      <c r="M76" s="9"/>
+      <c r="N76" s="9"/>
+      <c r="O76" s="9"/>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B77" s="11"/>
       <c r="C77" s="11"/>
@@ -4837,7 +4865,7 @@
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B78" s="11"/>
       <c r="C78" s="11"/>
@@ -4856,7 +4884,7 @@
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" s="11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B79" s="11"/>
       <c r="C79" s="11"/>
@@ -4875,7 +4903,7 @@
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" s="11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B80" s="11"/>
       <c r="C80" s="11"/>
@@ -4894,7 +4922,7 @@
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" s="11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B81" s="11"/>
       <c r="C81" s="11"/>
@@ -4913,7 +4941,7 @@
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B82" s="11"/>
       <c r="C82" s="11"/>
@@ -4932,7 +4960,7 @@
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B83" s="11"/>
       <c r="C83" s="11"/>
@@ -4951,7 +4979,7 @@
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" s="11" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B84" s="11"/>
       <c r="C84" s="11"/>
@@ -4970,7 +4998,7 @@
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" s="11" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B85" s="11"/>
       <c r="C85" s="11"/>
@@ -4989,7 +5017,7 @@
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" s="11" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B86" s="11"/>
       <c r="C86" s="11"/>
@@ -5008,7 +5036,7 @@
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B87" s="11"/>
       <c r="C87" s="11"/>
@@ -5027,7 +5055,7 @@
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B88" s="11"/>
       <c r="C88" s="11"/>
@@ -5044,32 +5072,51 @@
       <c r="N88" s="11"/>
       <c r="O88" s="11"/>
     </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A89" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B89" s="11"/>
+      <c r="C89" s="11"/>
+      <c r="D89" s="11"/>
+      <c r="E89" s="11"/>
+      <c r="F89" s="11"/>
+      <c r="G89" s="11"/>
+      <c r="H89" s="11"/>
+      <c r="I89" s="11"/>
+      <c r="J89" s="11"/>
+      <c r="K89" s="11"/>
+      <c r="L89" s="11"/>
+      <c r="M89" s="11"/>
+      <c r="N89" s="11"/>
+      <c r="O89" s="11"/>
+    </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="A85:O85"/>
-    <mergeCell ref="A87:O87"/>
+    <mergeCell ref="A86:O86"/>
     <mergeCell ref="A88:O88"/>
-    <mergeCell ref="A80:O80"/>
+    <mergeCell ref="A89:O89"/>
     <mergeCell ref="A81:O81"/>
     <mergeCell ref="A82:O82"/>
     <mergeCell ref="A83:O83"/>
     <mergeCell ref="A84:O84"/>
-    <mergeCell ref="A86:O86"/>
-    <mergeCell ref="A75:O75"/>
+    <mergeCell ref="A85:O85"/>
+    <mergeCell ref="A87:O87"/>
     <mergeCell ref="A76:O76"/>
     <mergeCell ref="A77:O77"/>
     <mergeCell ref="A78:O78"/>
     <mergeCell ref="A79:O79"/>
-    <mergeCell ref="A70:O70"/>
+    <mergeCell ref="A80:O80"/>
     <mergeCell ref="A71:O71"/>
     <mergeCell ref="A72:O72"/>
     <mergeCell ref="A73:O73"/>
     <mergeCell ref="A74:O74"/>
-    <mergeCell ref="A65:O65"/>
+    <mergeCell ref="A75:O75"/>
     <mergeCell ref="A66:O66"/>
     <mergeCell ref="A67:O67"/>
     <mergeCell ref="A68:O68"/>
     <mergeCell ref="A69:O69"/>
+    <mergeCell ref="A70:O70"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="A2:O2"/>
     <mergeCell ref="A3:O3"/>

</xml_diff>